<commit_message>
Updated some system test cases(preliminary).
</commit_message>
<xml_diff>
--- a/TECH/TEST/ST/WORK IN PROGRESS/SWSYS_TS.xlsx
+++ b/TECH/TEST/ST/WORK IN PROGRESS/SWSYS_TS.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="286">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="317">
   <si>
     <t>SERIS</t>
   </si>
@@ -302,20 +302,9 @@
     <t>Testing authentication of user into the system</t>
   </si>
   <si>
-    <t>Screen with list of users and their 
-responsible stations will be displayed.</t>
-  </si>
-  <si>
     <t>Viewing individual persona</t>
   </si>
   <si>
-    <t>Viewing all users' personas</t>
-  </si>
-  <si>
-    <t>A pop-up menu with information on 
-respective person's persona information should be displayed.</t>
-  </si>
-  <si>
     <t>Adding station for particular person</t>
   </si>
   <si>
@@ -325,14 +314,6 @@
     <t>Removing station from particular person</t>
   </si>
   <si>
-    <t>A new station should be added inside 
-the list of stations.</t>
-  </si>
-  <si>
-    <t>Press (x)  from station icon from
- the station lists.</t>
-  </si>
-  <si>
     <t>T3.2</t>
   </si>
   <si>
@@ -447,12 +428,6 @@
     <t>T7.2</t>
   </si>
   <si>
-    <t>T7.3</t>
-  </si>
-  <si>
-    <t>T7.4</t>
-  </si>
-  <si>
     <t>T8.2</t>
   </si>
   <si>
@@ -618,10 +593,6 @@
     <t>T3.6</t>
   </si>
   <si>
-    <t>Alert message for confirmation should be popped up. If confirmed "yes",that particular station should be removed
- from the list.</t>
-  </si>
-  <si>
     <t>Change access right</t>
   </si>
   <si>
@@ -646,33 +617,7 @@
     <t>Select a particular device under a particular user</t>
   </si>
   <si>
-    <t>View list of existing personas</t>
-  </si>
-  <si>
-    <t>Select a particular persona for updating its information</t>
-  </si>
-  <si>
     <t>Sending data from device to AWS cloud IoT core</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Pre-condition: Assume system user with admin-right has already logged into the system.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Admin-user clicks on persona tab. </t>
-    </r>
-  </si>
-  <si>
-    <t>Admin-user click on a particular user name 
-from the list of personas.</t>
   </si>
   <si>
     <t>Checking construction of structured data from incoming
@@ -734,19 +679,12 @@
  have been updated.</t>
   </si>
   <si>
-    <t>Go to suers page and click on any user.</t>
-  </si>
-  <si>
     <t>Information of that user should be able to view.</t>
   </si>
   <si>
     <t>1) Go to users page and click on any user and 
 update with new password in password field of that particular user's information and save.
 2) User log out from the system and log in again using new password.</t>
-  </si>
-  <si>
-    <t>Key in new station name in the name field of the persona page.
-Press "Add Station" button.</t>
   </si>
   <si>
     <r>
@@ -855,46 +793,9 @@
  the device list anymore.</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Pre-condition: Assume system user with 
-admin-right has already logged into the system.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-1)  Go to user list page.</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-  </si>
-  <si>
-    <t>List of users should be able to see.</t>
-  </si>
-  <si>
     <t>Deactivate account</t>
   </si>
   <si>
-    <t>Testing on View/select persona</t>
-  </si>
-  <si>
     <t>Testing on Select device(s)</t>
   </si>
   <si>
@@ -902,10 +803,6 @@
   </si>
   <si>
     <t>Testing on Sending data</t>
-  </si>
-  <si>
-    <t>1) User's information of that particular should be
-available for viewing.</t>
   </si>
   <si>
     <t>Device's information should be available for viewing.</t>
@@ -923,36 +820,6 @@
   <si>
     <t>It should display respective device page with 
 all the information.</t>
-  </si>
-  <si>
-    <t>It should display list of persons with associated 
-stations under their care/responsibility.</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Pre-condition: Assume  user with 
-admin-right has already logged into the system.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Go to personas page and check the screen.</t>
-    </r>
   </si>
   <si>
     <t xml:space="preserve"> Select a device under device list page.</t>
@@ -989,13 +856,6 @@
     </r>
   </si>
   <si>
-    <t>1) Select a persona from the list under personas page.</t>
-  </si>
-  <si>
-    <t>It should display respective persona page and 
-associated information.</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">Pre-condition: Make sure that the systen is up and running, and able to send out data from sensors and devices 
 </t>
@@ -1111,6 +971,232 @@
   </si>
   <si>
     <t>Draft version</t>
+  </si>
+  <si>
+    <t>3.1..3.1</t>
+  </si>
+  <si>
+    <t>Remark</t>
+  </si>
+  <si>
+    <t>T26</t>
+  </si>
+  <si>
+    <t>T26.1</t>
+  </si>
+  <si>
+    <t>T26.2</t>
+  </si>
+  <si>
+    <t>T26.3</t>
+  </si>
+  <si>
+    <t>Login using particular password.</t>
+  </si>
+  <si>
+    <t>The user should be able to login.</t>
+  </si>
+  <si>
+    <t>Current user logout from the system.</t>
+  </si>
+  <si>
+    <t>The user should logout from the system</t>
+  </si>
+  <si>
+    <t>T26.4</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>The user opens the browser again using the web link(EC2).</t>
+  </si>
+  <si>
+    <t>Testing for confirmation of actual logout for a particular user.</t>
+  </si>
+  <si>
+    <t>Testing on Login.</t>
+  </si>
+  <si>
+    <t>Testing on  Logout</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User login again using his own credential. 
+User  closes the browser without logging out.
+</t>
+  </si>
+  <si>
+    <t>It should be in main login page requesting user ID and password again. It should not be 
+in dashboard page and the use should have not been logged in. Otherwise, test fails.</t>
+  </si>
+  <si>
+    <t>Testing on refreshing  the page</t>
+  </si>
+  <si>
+    <t>After login, navigate the pages (dashboard, users, stations, etc.), 
+and then press  refresh button from the browser.</t>
+  </si>
+  <si>
+    <t>The browser should stay in current page with updated data after refreshing. It shouldn't have any errors. Otherwise, test fails.</t>
+  </si>
+  <si>
+    <t>Checking security behavior( Login and Logout)
+(Non-Functional)</t>
+  </si>
+  <si>
+    <t>Viewing users' personas</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Pre-condition: Assume system user with admin-right has already logged into the system.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>User presses it account on user page.
+User clicks on persona drop-down list.</t>
+    </r>
+  </si>
+  <si>
+    <t>List of available  personas should be displayed in the drop-down list.</t>
+  </si>
+  <si>
+    <t>It should go to respective page of particular user. The  user's persona information should be displayed.</t>
+  </si>
+  <si>
+    <t>Admin-user click on a particular user name 
+from the list of users from user page.</t>
+  </si>
+  <si>
+    <t>It seems there is problem in handling data in cloud cache.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Pre-condition: Assume system user with 
+admin-right has already logged into the system.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+1)  Go to user page and check the list.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+  </si>
+  <si>
+    <t>List of users should be able to be viewed.</t>
+  </si>
+  <si>
+    <t>1) Updated information of that particular user should be available for viewing.</t>
+  </si>
+  <si>
+    <t>"There was an unexpected error (type=Not Found, status=404)."
+Page showed error!</t>
+  </si>
+  <si>
+    <t>No device list found!</t>
+  </si>
+  <si>
+    <t>No option for adding device found!</t>
+  </si>
+  <si>
+    <t>No option found for viewing device!</t>
+  </si>
+  <si>
+    <t>Go to users page and click on a particular user.</t>
+  </si>
+  <si>
+    <t>Checking history record</t>
+  </si>
+  <si>
+    <t>Testing on history record data</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Assumption: The system already have some data relating to users, stations, etc in backend database.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Go to history record page and view the record in graph.</t>
+    </r>
+  </si>
+  <si>
+    <t>There should be relavent data displayed in graph.</t>
+  </si>
+  <si>
+    <t>Checking on automatic update of history record after editing and navigation</t>
+  </si>
+  <si>
+    <t>Edit any station name from station page and save it.
+Navigate back to history record page</t>
+  </si>
+  <si>
+    <t>.It should have fetched newly updated data and 
+display it correctly. Otherwise, test fails.</t>
+  </si>
+  <si>
+    <t>T2.5</t>
+  </si>
+  <si>
+    <t>Creating new station</t>
+  </si>
+  <si>
+    <t>Are there any manual processes needed to be done
+ like setting rules from AWS IoT core?</t>
+  </si>
+  <si>
+    <t>Click on a particular user name from the list of users from user page. Press "Select" button for adding new stations for the user and save.
+Press "Save" button.</t>
+  </si>
+  <si>
+    <t>New stations should have been added for the user. Otherwise, test fails.</t>
+  </si>
+  <si>
+    <t>Click on a particular user name from the list of users from user page. Press (x)  beside station icon and save.</t>
+  </si>
+  <si>
+    <t>Alert message for confirmation should be popped up. If confirmed "yes",that particular station should be removed from the list.</t>
+  </si>
+  <si>
+    <t>Request message should be popped up for confirmation of removal.</t>
+  </si>
+  <si>
+    <t>A new station should have been added in the station list.</t>
+  </si>
+  <si>
+    <t>Navigate to Station page and press "Add" button.
+Key in new station name in the name field of the page and other information. Check and verify by navigating to station page.</t>
   </si>
 </sst>
 </file>
@@ -1394,7 +1480,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1466,13 +1552,18 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1481,20 +1572,35 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1529,7 +1635,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns="" xmlns:wpc="http://schemas.microsoft.com/office/word/2010/wordprocessingCanvas" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:cx2="http://schemas.microsoft.com/office/drawing/2015/10/21/chartex" xmlns:cx3="http://schemas.microsoft.com/office/drawing/2016/5/9/chartex" xmlns:cx4="http://schemas.microsoft.com/office/drawing/2016/5/10/chartex" xmlns:cx5="http://schemas.microsoft.com/office/drawing/2016/5/11/chartex" xmlns:cx6="http://schemas.microsoft.com/office/drawing/2016/5/12/chartex" xmlns:cx7="http://schemas.microsoft.com/office/drawing/2016/5/13/chartex" xmlns:cx8="http://schemas.microsoft.com/office/drawing/2016/5/14/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:aink="http://schemas.microsoft.com/office/drawing/2016/ink" xmlns:am3d="http://schemas.microsoft.com/office/drawing/2017/model3d" xmlns:o="urn:schemas-microsoft-com:office:office" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:wp14="http://schemas.microsoft.com/office/word/2010/wordprocessingDrawing" xmlns:wp="http://schemas.openxmlformats.org/drawingml/2006/wordprocessingDrawing" xmlns:w10="urn:schemas-microsoft-com:office:word" xmlns:w="http://schemas.openxmlformats.org/wordprocessingml/2006/main" xmlns:w14="http://schemas.microsoft.com/office/word/2010/wordml" xmlns:w15="http://schemas.microsoft.com/office/word/2012/wordml" xmlns:w16cid="http://schemas.microsoft.com/office/word/2016/wordml/cid" xmlns:w16se="http://schemas.microsoft.com/office/word/2015/wordml/symex" xmlns:wpg="http://schemas.microsoft.com/office/word/2010/wordprocessingGroup" xmlns:wpi="http://schemas.microsoft.com/office/word/2010/wordprocessingInk" xmlns:wne="http://schemas.microsoft.com/office/word/2006/wordml" xmlns:wps="http://schemas.microsoft.com/office/word/2010/wordprocessingShape" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:pic="http://schemas.openxmlformats.org/drawingml/2006/picture" xmlns:lc="http://schemas.openxmlformats.org/drawingml/2006/lockedCanvas" val="0"/>
+              <a14:useLocalDpi xmlns:lc="http://schemas.openxmlformats.org/drawingml/2006/lockedCanvas" xmlns:pic="http://schemas.openxmlformats.org/drawingml/2006/picture" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:wps="http://schemas.microsoft.com/office/word/2010/wordprocessingShape" xmlns:wne="http://schemas.microsoft.com/office/word/2006/wordml" xmlns:wpi="http://schemas.microsoft.com/office/word/2010/wordprocessingInk" xmlns:wpg="http://schemas.microsoft.com/office/word/2010/wordprocessingGroup" xmlns:w16se="http://schemas.microsoft.com/office/word/2015/wordml/symex" xmlns:w16cid="http://schemas.microsoft.com/office/word/2016/wordml/cid" xmlns:w15="http://schemas.microsoft.com/office/word/2012/wordml" xmlns:w14="http://schemas.microsoft.com/office/word/2010/wordml" xmlns:w="http://schemas.openxmlformats.org/wordprocessingml/2006/main" xmlns:w10="urn:schemas-microsoft-com:office:word" xmlns:wp="http://schemas.openxmlformats.org/drawingml/2006/wordprocessingDrawing" xmlns:wp14="http://schemas.microsoft.com/office/word/2010/wordprocessingDrawing" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:o="urn:schemas-microsoft-com:office:office" xmlns:am3d="http://schemas.microsoft.com/office/drawing/2017/model3d" xmlns:aink="http://schemas.microsoft.com/office/drawing/2016/ink" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:cx8="http://schemas.microsoft.com/office/drawing/2016/5/14/chartex" xmlns:cx7="http://schemas.microsoft.com/office/drawing/2016/5/13/chartex" xmlns:cx6="http://schemas.microsoft.com/office/drawing/2016/5/12/chartex" xmlns:cx5="http://schemas.microsoft.com/office/drawing/2016/5/11/chartex" xmlns:cx4="http://schemas.microsoft.com/office/drawing/2016/5/10/chartex" xmlns:cx3="http://schemas.microsoft.com/office/drawing/2016/5/9/chartex" xmlns:cx2="http://schemas.microsoft.com/office/drawing/2015/10/21/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:wpc="http://schemas.microsoft.com/office/word/2010/wordprocessingCanvas" xmlns="" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -1895,7 +2001,7 @@
         <v>3</v>
       </c>
       <c r="B14" t="s">
-        <v>260</v>
+        <v>238</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -1936,7 +2042,7 @@
         <v>84</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>285</v>
+        <v>263</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -2100,10 +2206,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:R109"/>
+  <dimension ref="A1:R112"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G101" sqref="G101"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2111,12 +2217,13 @@
     <col min="1" max="1" width="8.28515625" customWidth="1"/>
     <col min="2" max="2" width="37.5703125" customWidth="1"/>
     <col min="3" max="3" width="13.42578125" customWidth="1"/>
-    <col min="4" max="4" width="53.42578125" customWidth="1"/>
+    <col min="4" max="4" width="75.28515625" customWidth="1"/>
     <col min="5" max="5" width="11.140625" customWidth="1"/>
     <col min="6" max="6" width="10.85546875" customWidth="1"/>
-    <col min="7" max="7" width="63.28515625" customWidth="1"/>
-    <col min="8" max="8" width="47.85546875" customWidth="1"/>
-    <col min="9" max="9" width="18.140625" customWidth="1"/>
+    <col min="7" max="7" width="66.85546875" customWidth="1"/>
+    <col min="8" max="8" width="54.28515625" customWidth="1"/>
+    <col min="9" max="9" width="20" customWidth="1"/>
+    <col min="10" max="10" width="68.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18">
@@ -2146,6 +2253,9 @@
       </c>
       <c r="I1" s="10" t="s">
         <v>33</v>
+      </c>
+      <c r="J1" s="10" t="s">
+        <v>265</v>
       </c>
       <c r="P1" s="18" t="s">
         <v>35</v>
@@ -2169,12 +2279,13 @@
       <c r="I2" s="12" t="s">
         <v>44</v>
       </c>
+      <c r="J2" s="3"/>
     </row>
     <row r="3" spans="1:18" ht="57.75" customHeight="1">
-      <c r="A3" s="39" t="s">
+      <c r="A3" s="47" t="s">
         <v>47</v>
       </c>
-      <c r="B3" s="41" t="s">
+      <c r="B3" s="42" t="s">
         <v>86</v>
       </c>
       <c r="C3" s="19" t="s">
@@ -2194,12 +2305,13 @@
         <v>73</v>
       </c>
       <c r="I3" s="14" t="s">
-        <v>45</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="J3" s="3"/>
     </row>
     <row r="4" spans="1:18" ht="38.25" customHeight="1">
-      <c r="A4" s="40"/>
-      <c r="B4" s="42"/>
+      <c r="A4" s="48"/>
+      <c r="B4" s="45"/>
       <c r="C4" s="19" t="s">
         <v>36</v>
       </c>
@@ -2217,12 +2329,13 @@
         <v>83</v>
       </c>
       <c r="I4" s="14" t="s">
-        <v>45</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="J4" s="3"/>
     </row>
     <row r="5" spans="1:18" ht="45" customHeight="1">
-      <c r="A5" s="40"/>
-      <c r="B5" s="42"/>
+      <c r="A5" s="48"/>
+      <c r="B5" s="45"/>
       <c r="C5" s="19" t="s">
         <v>37</v>
       </c>
@@ -2240,12 +2353,13 @@
         <v>82</v>
       </c>
       <c r="I5" s="14" t="s">
-        <v>45</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="J5" s="3"/>
     </row>
     <row r="6" spans="1:18" ht="38.25" customHeight="1">
-      <c r="A6" s="40"/>
-      <c r="B6" s="43"/>
+      <c r="A6" s="48"/>
+      <c r="B6" s="46"/>
       <c r="C6" s="19" t="s">
         <v>72</v>
       </c>
@@ -2263,425 +2377,472 @@
         <v>82</v>
       </c>
       <c r="I6" s="14" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18" ht="78.75" customHeight="1">
-      <c r="A7" s="45" t="s">
+        <v>35</v>
+      </c>
+      <c r="J6" s="3"/>
+    </row>
+    <row r="7" spans="1:18" ht="105" customHeight="1">
+      <c r="A7" s="39" t="s">
         <v>48</v>
       </c>
-      <c r="B7" s="41" t="s">
+      <c r="B7" s="42" t="s">
         <v>85</v>
       </c>
       <c r="C7" s="20" t="s">
         <v>38</v>
       </c>
       <c r="D7" s="24" t="s">
-        <v>89</v>
+        <v>286</v>
       </c>
       <c r="E7" s="3"/>
       <c r="F7" s="3">
         <v>1</v>
       </c>
       <c r="G7" s="23" t="s">
-        <v>203</v>
+        <v>287</v>
       </c>
       <c r="H7" s="13" t="s">
-        <v>87</v>
+        <v>288</v>
       </c>
       <c r="I7" s="14" t="s">
-        <v>45</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="J7" s="3"/>
       <c r="P7" s="18"/>
       <c r="Q7" s="18"/>
       <c r="R7" s="18"/>
     </row>
-    <row r="8" spans="1:18" ht="48.75" customHeight="1">
-      <c r="A8" s="46"/>
-      <c r="B8" s="42"/>
+    <row r="8" spans="1:18" ht="69.75" customHeight="1">
+      <c r="A8" s="43"/>
+      <c r="B8" s="45"/>
       <c r="C8" s="20" t="s">
         <v>39</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E8" s="3"/>
       <c r="F8" s="3">
         <v>1</v>
       </c>
       <c r="G8" s="13" t="s">
-        <v>204</v>
+        <v>290</v>
       </c>
       <c r="H8" s="13" t="s">
-        <v>90</v>
+        <v>289</v>
       </c>
       <c r="I8" s="14" t="s">
-        <v>45</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="J8" s="3"/>
       <c r="P8" s="18"/>
       <c r="Q8" s="18"/>
       <c r="R8" s="18"/>
     </row>
-    <row r="9" spans="1:18" ht="60.75" customHeight="1">
-      <c r="A9" s="46"/>
-      <c r="B9" s="42"/>
+    <row r="9" spans="1:18" ht="105.75" customHeight="1">
+      <c r="A9" s="43"/>
+      <c r="B9" s="45"/>
       <c r="C9" s="20" t="s">
         <v>46</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="E9" s="3"/>
       <c r="F9" s="3">
         <v>1</v>
       </c>
       <c r="G9" s="13" t="s">
-        <v>220</v>
+        <v>310</v>
       </c>
       <c r="H9" s="13" t="s">
-        <v>94</v>
+        <v>311</v>
       </c>
       <c r="I9" s="14" t="s">
-        <v>45</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="J9" s="13"/>
       <c r="P9" s="18"/>
       <c r="Q9" s="18"/>
       <c r="R9" s="18"/>
     </row>
-    <row r="10" spans="1:18" ht="66.75" customHeight="1">
-      <c r="A10" s="44"/>
-      <c r="B10" s="44"/>
+    <row r="10" spans="1:18" ht="83.25" customHeight="1">
+      <c r="A10" s="57"/>
+      <c r="B10" s="57"/>
       <c r="C10" s="20" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="E10" s="3"/>
       <c r="F10" s="3">
         <v>1</v>
       </c>
       <c r="G10" s="13" t="s">
-        <v>95</v>
+        <v>312</v>
       </c>
       <c r="H10" s="13" t="s">
-        <v>191</v>
+        <v>313</v>
       </c>
       <c r="I10" s="14" t="s">
-        <v>45</v>
+        <v>35</v>
+      </c>
+      <c r="J10" s="3" t="s">
+        <v>314</v>
       </c>
       <c r="P10" s="18"/>
       <c r="Q10" s="18"/>
       <c r="R10" s="18"/>
     </row>
-    <row r="11" spans="1:18" ht="74.25" customHeight="1">
-      <c r="A11" s="45" t="s">
-        <v>49</v>
-      </c>
-      <c r="B11" s="41" t="s">
-        <v>225</v>
-      </c>
+    <row r="11" spans="1:18" ht="66.75" customHeight="1">
+      <c r="A11" s="49"/>
+      <c r="B11" s="49"/>
       <c r="C11" s="20" t="s">
-        <v>212</v>
+        <v>307</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>210</v>
+        <v>308</v>
       </c>
       <c r="E11" s="3"/>
       <c r="F11" s="3">
         <v>1</v>
       </c>
-      <c r="G11" s="22" t="s">
-        <v>214</v>
+      <c r="G11" s="13" t="s">
+        <v>316</v>
       </c>
       <c r="H11" s="13" t="s">
-        <v>213</v>
+        <v>315</v>
       </c>
       <c r="I11" s="14" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="12" spans="1:18" ht="91.5" customHeight="1">
-      <c r="A12" s="46"/>
-      <c r="B12" s="42"/>
+        <v>35</v>
+      </c>
+      <c r="J11" s="13" t="s">
+        <v>309</v>
+      </c>
+      <c r="P11" s="18"/>
+      <c r="Q11" s="18"/>
+      <c r="R11" s="18"/>
+    </row>
+    <row r="12" spans="1:18" ht="85.5" customHeight="1">
+      <c r="A12" s="39" t="s">
+        <v>49</v>
+      </c>
+      <c r="B12" s="42" t="s">
+        <v>211</v>
+      </c>
       <c r="C12" s="20" t="s">
-        <v>96</v>
+        <v>200</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>211</v>
-      </c>
-      <c r="E12" s="3"/>
+        <v>198</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>264</v>
+      </c>
       <c r="F12" s="3">
         <v>1</v>
       </c>
-      <c r="G12" s="13" t="s">
-        <v>215</v>
+      <c r="G12" s="22" t="s">
+        <v>202</v>
       </c>
       <c r="H12" s="13" t="s">
-        <v>216</v>
+        <v>201</v>
       </c>
       <c r="I12" s="14" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="13" spans="1:18" ht="37.5" customHeight="1">
-      <c r="A13" s="46"/>
-      <c r="B13" s="42"/>
+        <v>35</v>
+      </c>
+      <c r="J12" s="3"/>
+    </row>
+    <row r="13" spans="1:18" ht="91.5" customHeight="1">
+      <c r="A13" s="43"/>
+      <c r="B13" s="45"/>
       <c r="C13" s="20" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="E13" s="3"/>
+        <v>199</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>264</v>
+      </c>
       <c r="F13" s="3">
         <v>1</v>
       </c>
-      <c r="G13" s="3" t="s">
-        <v>217</v>
-      </c>
-      <c r="H13" s="3" t="s">
-        <v>218</v>
+      <c r="G13" s="13" t="s">
+        <v>203</v>
+      </c>
+      <c r="H13" s="13" t="s">
+        <v>204</v>
       </c>
       <c r="I13" s="14" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="14" spans="1:18" ht="84.75" customHeight="1">
-      <c r="A14" s="46"/>
-      <c r="B14" s="42"/>
+        <v>35</v>
+      </c>
+      <c r="J13" s="3"/>
+    </row>
+    <row r="14" spans="1:18" ht="37.5" customHeight="1">
+      <c r="A14" s="43"/>
+      <c r="B14" s="45"/>
       <c r="C14" s="20" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>188</v>
-      </c>
-      <c r="E14" s="3"/>
+        <v>180</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>264</v>
+      </c>
       <c r="F14" s="3">
         <v>1</v>
       </c>
-      <c r="G14" s="13" t="s">
-        <v>219</v>
-      </c>
-      <c r="H14" s="13" t="s">
-        <v>259</v>
+      <c r="G14" s="3" t="s">
+        <v>299</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>205</v>
       </c>
       <c r="I14" s="14" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="15" spans="1:18" ht="126" customHeight="1">
-      <c r="A15" s="46"/>
-      <c r="B15" s="42"/>
+        <v>35</v>
+      </c>
+      <c r="J14" s="3"/>
+    </row>
+    <row r="15" spans="1:18" ht="84.75" customHeight="1">
+      <c r="A15" s="43"/>
+      <c r="B15" s="45"/>
       <c r="C15" s="20" t="s">
-        <v>189</v>
+        <v>93</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>192</v>
+        <v>181</v>
       </c>
       <c r="E15" s="3"/>
       <c r="F15" s="3">
         <v>1</v>
       </c>
       <c r="G15" s="13" t="s">
-        <v>221</v>
+        <v>206</v>
       </c>
       <c r="H15" s="13" t="s">
-        <v>222</v>
+        <v>237</v>
       </c>
       <c r="I15" s="14" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="16" spans="1:18" ht="126.75" customHeight="1">
-      <c r="A16" s="47"/>
-      <c r="B16" s="43"/>
+      <c r="J15" s="3"/>
+    </row>
+    <row r="16" spans="1:18" ht="126" customHeight="1">
+      <c r="A16" s="43"/>
+      <c r="B16" s="45"/>
       <c r="C16" s="20" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>236</v>
+        <v>184</v>
       </c>
       <c r="E16" s="3"/>
       <c r="F16" s="3">
         <v>1</v>
       </c>
       <c r="G16" s="13" t="s">
-        <v>223</v>
+        <v>207</v>
       </c>
       <c r="H16" s="13" t="s">
-        <v>224</v>
+        <v>208</v>
       </c>
       <c r="I16" s="14" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" ht="97.5" customHeight="1">
-      <c r="A17" s="45" t="s">
-        <v>50</v>
-      </c>
-      <c r="B17" s="41" t="s">
-        <v>209</v>
-      </c>
+      <c r="J16" s="3"/>
+    </row>
+    <row r="17" spans="1:10" ht="126.75" customHeight="1">
+      <c r="A17" s="44"/>
+      <c r="B17" s="46"/>
       <c r="C17" s="20" t="s">
-        <v>99</v>
+        <v>183</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>193</v>
+        <v>220</v>
       </c>
       <c r="E17" s="3"/>
       <c r="F17" s="3">
         <v>1</v>
       </c>
       <c r="G17" s="13" t="s">
-        <v>226</v>
+        <v>209</v>
       </c>
       <c r="H17" s="13" t="s">
-        <v>227</v>
+        <v>210</v>
       </c>
       <c r="I17" s="14" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" ht="85.5" customHeight="1">
-      <c r="A18" s="46"/>
-      <c r="B18" s="42"/>
+      <c r="J17" s="3"/>
+    </row>
+    <row r="18" spans="1:10" ht="117.75" customHeight="1">
+      <c r="A18" s="39" t="s">
+        <v>50</v>
+      </c>
+      <c r="B18" s="42" t="s">
+        <v>197</v>
+      </c>
       <c r="C18" s="20" t="s">
-        <v>124</v>
+        <v>94</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>194</v>
+        <v>185</v>
       </c>
       <c r="E18" s="3"/>
       <c r="F18" s="3">
         <v>1</v>
       </c>
       <c r="G18" s="13" t="s">
-        <v>229</v>
+        <v>212</v>
       </c>
       <c r="H18" s="13" t="s">
-        <v>230</v>
+        <v>213</v>
       </c>
       <c r="I18" s="14" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" ht="45.75" customHeight="1">
-      <c r="A19" s="46"/>
-      <c r="B19" s="42"/>
+      <c r="J18" s="3" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="85.5" customHeight="1">
+      <c r="A19" s="43"/>
+      <c r="B19" s="45"/>
       <c r="C19" s="20" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>228</v>
+        <v>186</v>
       </c>
       <c r="E19" s="3"/>
       <c r="F19" s="3">
         <v>1</v>
       </c>
       <c r="G19" s="13" t="s">
-        <v>231</v>
-      </c>
-      <c r="H19" s="3" t="s">
-        <v>242</v>
+        <v>215</v>
+      </c>
+      <c r="H19" s="13" t="s">
+        <v>216</v>
       </c>
       <c r="I19" s="14" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" ht="84" customHeight="1">
-      <c r="A20" s="47"/>
-      <c r="B20" s="43"/>
+      <c r="J19" s="3" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="45.75" customHeight="1">
+      <c r="A20" s="43"/>
+      <c r="B20" s="45"/>
       <c r="C20" s="20" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>195</v>
+        <v>214</v>
       </c>
       <c r="E20" s="3"/>
       <c r="F20" s="3">
         <v>1</v>
       </c>
       <c r="G20" s="13" t="s">
-        <v>232</v>
-      </c>
-      <c r="H20" s="13" t="s">
-        <v>233</v>
+        <v>217</v>
+      </c>
+      <c r="H20" s="3" t="s">
+        <v>224</v>
       </c>
       <c r="I20" s="14" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" ht="72.75" customHeight="1">
-      <c r="A21" s="45" t="s">
-        <v>51</v>
-      </c>
-      <c r="B21" s="41" t="s">
-        <v>239</v>
-      </c>
+      <c r="J20" s="3" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="100.5" customHeight="1">
+      <c r="A21" s="44"/>
+      <c r="B21" s="46"/>
       <c r="C21" s="20" t="s">
-        <v>100</v>
+        <v>121</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>196</v>
+        <v>187</v>
       </c>
       <c r="E21" s="3"/>
       <c r="F21" s="3">
-        <v>2</v>
-      </c>
-      <c r="G21" s="22" t="s">
-        <v>234</v>
-      </c>
-      <c r="H21" s="3" t="s">
-        <v>235</v>
+        <v>1</v>
+      </c>
+      <c r="G21" s="13" t="s">
+        <v>218</v>
+      </c>
+      <c r="H21" s="13" t="s">
+        <v>219</v>
       </c>
       <c r="I21" s="14" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" ht="81.75" customHeight="1">
-      <c r="A22" s="46"/>
-      <c r="B22" s="42"/>
+      <c r="J21" s="3" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="72.75" customHeight="1">
+      <c r="A22" s="39" t="s">
+        <v>51</v>
+      </c>
+      <c r="B22" s="42" t="s">
+        <v>222</v>
+      </c>
       <c r="C22" s="20" t="s">
-        <v>127</v>
+        <v>95</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
       <c r="E22" s="3"/>
       <c r="F22" s="3">
         <v>2</v>
       </c>
-      <c r="G22" s="13" t="s">
-        <v>243</v>
-      </c>
-      <c r="H22" s="13" t="s">
-        <v>241</v>
+      <c r="G22" s="22" t="s">
+        <v>292</v>
+      </c>
+      <c r="H22" s="3" t="s">
+        <v>293</v>
       </c>
       <c r="I22" s="14" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9">
-      <c r="A23" s="46"/>
-      <c r="B23" s="42"/>
+        <v>35</v>
+      </c>
+      <c r="J22" s="3"/>
+    </row>
+    <row r="23" spans="1:10" ht="95.25" customHeight="1">
+      <c r="A23" s="43"/>
+      <c r="B23" s="45"/>
       <c r="C23" s="20" t="s">
-        <v>128</v>
-      </c>
-      <c r="D23" s="3"/>
+        <v>122</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>189</v>
+      </c>
       <c r="E23" s="3"/>
-      <c r="F23" s="3"/>
-      <c r="G23" s="3"/>
-      <c r="H23" s="3"/>
+      <c r="F23" s="3">
+        <v>2</v>
+      </c>
+      <c r="G23" s="13" t="s">
+        <v>225</v>
+      </c>
+      <c r="H23" s="13" t="s">
+        <v>294</v>
+      </c>
       <c r="I23" s="14" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9">
-      <c r="A24" s="47"/>
-      <c r="B24" s="43"/>
+        <v>35</v>
+      </c>
+      <c r="J23" s="3"/>
+    </row>
+    <row r="24" spans="1:10">
+      <c r="A24" s="43"/>
+      <c r="B24" s="45"/>
       <c r="C24" s="20" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="D24" s="3"/>
       <c r="E24" s="3"/>
@@ -2691,73 +2852,79 @@
       <c r="I24" s="14" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="25" spans="1:9" ht="82.5" customHeight="1">
-      <c r="A25" s="45" t="s">
-        <v>52</v>
-      </c>
-      <c r="B25" s="41" t="s">
-        <v>238</v>
-      </c>
+      <c r="J24" s="3"/>
+    </row>
+    <row r="25" spans="1:10">
+      <c r="A25" s="44"/>
+      <c r="B25" s="46"/>
       <c r="C25" s="20" t="s">
-        <v>101</v>
-      </c>
-      <c r="D25" s="3" t="s">
-        <v>198</v>
-      </c>
+        <v>124</v>
+      </c>
+      <c r="D25" s="3"/>
       <c r="E25" s="3"/>
-      <c r="F25" s="3">
-        <v>1</v>
-      </c>
-      <c r="G25" s="22" t="s">
-        <v>249</v>
-      </c>
-      <c r="H25" s="13" t="s">
-        <v>244</v>
-      </c>
+      <c r="F25" s="3"/>
+      <c r="G25" s="3"/>
+      <c r="H25" s="3"/>
       <c r="I25" s="14" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="26" spans="1:9" ht="38.25" customHeight="1">
-      <c r="A26" s="46"/>
-      <c r="B26" s="42"/>
+      <c r="J25" s="3"/>
+    </row>
+    <row r="26" spans="1:10" ht="82.5" customHeight="1">
+      <c r="A26" s="39" t="s">
+        <v>52</v>
+      </c>
+      <c r="B26" s="42" t="s">
+        <v>221</v>
+      </c>
       <c r="C26" s="20" t="s">
-        <v>130</v>
+        <v>96</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
       <c r="E26" s="3"/>
       <c r="F26" s="3">
         <v>1</v>
       </c>
-      <c r="G26" s="3" t="s">
-        <v>248</v>
+      <c r="G26" s="22" t="s">
+        <v>229</v>
       </c>
       <c r="H26" s="13" t="s">
-        <v>245</v>
-      </c>
-      <c r="I26" s="14"/>
-    </row>
-    <row r="27" spans="1:9">
-      <c r="A27" s="46"/>
-      <c r="B27" s="42"/>
+        <v>226</v>
+      </c>
+      <c r="I26" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="J26" s="3"/>
+    </row>
+    <row r="27" spans="1:10" ht="38.25" customHeight="1">
+      <c r="A27" s="43"/>
+      <c r="B27" s="45"/>
       <c r="C27" s="20" t="s">
-        <v>131</v>
-      </c>
-      <c r="D27" s="3"/>
+        <v>125</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>191</v>
+      </c>
       <c r="E27" s="3"/>
-      <c r="F27" s="3"/>
-      <c r="G27" s="3"/>
-      <c r="H27" s="3"/>
+      <c r="F27" s="3">
+        <v>1</v>
+      </c>
+      <c r="G27" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="H27" s="13" t="s">
+        <v>227</v>
+      </c>
       <c r="I27" s="14"/>
-    </row>
-    <row r="28" spans="1:9" ht="23.25" customHeight="1">
-      <c r="A28" s="47"/>
-      <c r="B28" s="43"/>
+      <c r="J27" s="3"/>
+    </row>
+    <row r="28" spans="1:10">
+      <c r="A28" s="43"/>
+      <c r="B28" s="45"/>
       <c r="C28" s="20" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="D28" s="3"/>
       <c r="E28" s="3"/>
@@ -2765,107 +2932,119 @@
       <c r="G28" s="3"/>
       <c r="H28" s="3"/>
       <c r="I28" s="14"/>
-    </row>
-    <row r="29" spans="1:9" ht="60">
-      <c r="A29" s="45" t="s">
-        <v>53</v>
-      </c>
-      <c r="B29" s="41" t="s">
-        <v>237</v>
-      </c>
+      <c r="J28" s="3"/>
+    </row>
+    <row r="29" spans="1:10" ht="23.25" customHeight="1">
+      <c r="A29" s="44"/>
+      <c r="B29" s="46"/>
       <c r="C29" s="20" t="s">
-        <v>102</v>
-      </c>
-      <c r="D29" s="3" t="s">
-        <v>200</v>
-      </c>
+        <v>127</v>
+      </c>
+      <c r="D29" s="3"/>
       <c r="E29" s="3"/>
       <c r="F29" s="3"/>
-      <c r="G29" s="13" t="s">
-        <v>247</v>
-      </c>
-      <c r="H29" s="13" t="s">
-        <v>246</v>
-      </c>
-      <c r="I29" s="14" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" ht="34.5" customHeight="1">
-      <c r="A30" s="46"/>
-      <c r="B30" s="42"/>
+      <c r="G29" s="3"/>
+      <c r="H29" s="3"/>
+      <c r="I29" s="14"/>
+      <c r="J29" s="3"/>
+    </row>
+    <row r="30" spans="1:10" ht="94.5" customHeight="1">
+      <c r="A30" s="39" t="s">
+        <v>53</v>
+      </c>
+      <c r="B30" s="42" t="s">
+        <v>301</v>
+      </c>
       <c r="C30" s="20" t="s">
-        <v>133</v>
-      </c>
-      <c r="D30" s="3" t="s">
-        <v>201</v>
+        <v>97</v>
+      </c>
+      <c r="D30" s="50" t="s">
+        <v>300</v>
       </c>
       <c r="E30" s="3"/>
-      <c r="F30" s="3"/>
-      <c r="G30" s="3" t="s">
-        <v>250</v>
-      </c>
-      <c r="H30" s="13" t="s">
-        <v>251</v>
-      </c>
-      <c r="I30" s="14"/>
-    </row>
-    <row r="31" spans="1:9">
-      <c r="A31" s="46"/>
-      <c r="B31" s="42"/>
+      <c r="F30" s="3">
+        <v>1</v>
+      </c>
+      <c r="G30" s="56" t="s">
+        <v>302</v>
+      </c>
+      <c r="H30" s="3" t="s">
+        <v>303</v>
+      </c>
+      <c r="I30" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="J30" s="3"/>
+    </row>
+    <row r="31" spans="1:10" ht="70.5" customHeight="1">
+      <c r="A31" s="43"/>
+      <c r="B31" s="45"/>
       <c r="C31" s="20" t="s">
-        <v>134</v>
-      </c>
-      <c r="D31" s="3"/>
+        <v>128</v>
+      </c>
+      <c r="D31" s="50" t="s">
+        <v>304</v>
+      </c>
       <c r="E31" s="3"/>
-      <c r="F31" s="3"/>
-      <c r="G31" s="3"/>
-      <c r="H31" s="3"/>
-      <c r="I31" s="14"/>
-    </row>
-    <row r="32" spans="1:9">
-      <c r="A32" s="47"/>
-      <c r="B32" s="43"/>
+      <c r="F31" s="3">
+        <v>2</v>
+      </c>
+      <c r="G31" s="13" t="s">
+        <v>305</v>
+      </c>
+      <c r="H31" s="13" t="s">
+        <v>306</v>
+      </c>
+      <c r="I31" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="J31" s="3"/>
+    </row>
+    <row r="32" spans="1:10" ht="114" customHeight="1">
+      <c r="A32" s="39" t="s">
+        <v>54</v>
+      </c>
+      <c r="B32" s="42" t="s">
+        <v>223</v>
+      </c>
       <c r="C32" s="20" t="s">
-        <v>135</v>
-      </c>
-      <c r="D32" s="3"/>
+        <v>98</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>192</v>
+      </c>
       <c r="E32" s="3"/>
       <c r="F32" s="3"/>
-      <c r="G32" s="3"/>
-      <c r="H32" s="3"/>
-      <c r="I32" s="14"/>
-    </row>
-    <row r="33" spans="1:9" ht="101.25" customHeight="1">
-      <c r="A33" s="45" t="s">
-        <v>54</v>
-      </c>
-      <c r="B33" s="41" t="s">
-        <v>240</v>
-      </c>
+      <c r="G32" s="22" t="s">
+        <v>230</v>
+      </c>
+      <c r="H32" s="13" t="s">
+        <v>231</v>
+      </c>
+      <c r="I32" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="J32" s="3"/>
+    </row>
+    <row r="33" spans="1:10">
+      <c r="A33" s="43"/>
+      <c r="B33" s="45"/>
       <c r="C33" s="20" t="s">
-        <v>103</v>
-      </c>
-      <c r="D33" s="3" t="s">
-        <v>202</v>
-      </c>
+        <v>129</v>
+      </c>
+      <c r="D33" s="3"/>
       <c r="E33" s="3"/>
       <c r="F33" s="3"/>
-      <c r="G33" s="22" t="s">
-        <v>252</v>
-      </c>
-      <c r="H33" s="13" t="s">
-        <v>253</v>
-      </c>
-      <c r="I33" s="14" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9">
-      <c r="A34" s="46"/>
-      <c r="B34" s="42"/>
+      <c r="G33" s="3"/>
+      <c r="H33" s="3"/>
+      <c r="I33" s="14"/>
+      <c r="J33" s="3"/>
+    </row>
+    <row r="34" spans="1:10">
+      <c r="A34" s="43"/>
+      <c r="B34" s="45"/>
       <c r="C34" s="20" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="D34" s="3"/>
       <c r="E34" s="3"/>
@@ -2873,12 +3052,13 @@
       <c r="G34" s="3"/>
       <c r="H34" s="3"/>
       <c r="I34" s="14"/>
-    </row>
-    <row r="35" spans="1:9">
-      <c r="A35" s="46"/>
-      <c r="B35" s="42"/>
+      <c r="J34" s="3"/>
+    </row>
+    <row r="35" spans="1:10">
+      <c r="A35" s="44"/>
+      <c r="B35" s="46"/>
       <c r="C35" s="20" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="D35" s="3"/>
       <c r="E35" s="3"/>
@@ -2886,46 +3066,49 @@
       <c r="G35" s="3"/>
       <c r="H35" s="3"/>
       <c r="I35" s="14"/>
-    </row>
-    <row r="36" spans="1:9">
-      <c r="A36" s="47"/>
-      <c r="B36" s="43"/>
+      <c r="J35" s="3"/>
+    </row>
+    <row r="36" spans="1:10" ht="30">
+      <c r="A36" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="B36" s="42" t="s">
+        <v>246</v>
+      </c>
       <c r="C36" s="20" t="s">
-        <v>138</v>
-      </c>
-      <c r="D36" s="3"/>
+        <v>99</v>
+      </c>
+      <c r="D36" s="13" t="s">
+        <v>193</v>
+      </c>
       <c r="E36" s="3"/>
       <c r="F36" s="3"/>
       <c r="G36" s="3"/>
       <c r="H36" s="3"/>
-      <c r="I36" s="14"/>
-    </row>
-    <row r="37" spans="1:9" ht="30">
-      <c r="A37" s="45" t="s">
-        <v>55</v>
-      </c>
-      <c r="B37" s="41" t="s">
-        <v>268</v>
-      </c>
+      <c r="I36" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="J36" s="3"/>
+    </row>
+    <row r="37" spans="1:10">
+      <c r="A37" s="43"/>
+      <c r="B37" s="45"/>
       <c r="C37" s="20" t="s">
-        <v>104</v>
-      </c>
-      <c r="D37" s="13" t="s">
-        <v>205</v>
-      </c>
+        <v>132</v>
+      </c>
+      <c r="D37" s="3"/>
       <c r="E37" s="3"/>
       <c r="F37" s="3"/>
       <c r="G37" s="3"/>
       <c r="H37" s="3"/>
-      <c r="I37" s="14" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9">
-      <c r="A38" s="46"/>
-      <c r="B38" s="42"/>
+      <c r="I37" s="14"/>
+      <c r="J37" s="3"/>
+    </row>
+    <row r="38" spans="1:10">
+      <c r="A38" s="43"/>
+      <c r="B38" s="45"/>
       <c r="C38" s="20" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="D38" s="3"/>
       <c r="E38" s="3"/>
@@ -2933,12 +3116,13 @@
       <c r="G38" s="3"/>
       <c r="H38" s="3"/>
       <c r="I38" s="14"/>
-    </row>
-    <row r="39" spans="1:9">
-      <c r="A39" s="46"/>
-      <c r="B39" s="42"/>
+      <c r="J38" s="3"/>
+    </row>
+    <row r="39" spans="1:10">
+      <c r="A39" s="44"/>
+      <c r="B39" s="46"/>
       <c r="C39" s="20" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="D39" s="3"/>
       <c r="E39" s="3"/>
@@ -2946,46 +3130,49 @@
       <c r="G39" s="3"/>
       <c r="H39" s="3"/>
       <c r="I39" s="14"/>
-    </row>
-    <row r="40" spans="1:9">
-      <c r="A40" s="47"/>
-      <c r="B40" s="43"/>
+      <c r="J39" s="3"/>
+    </row>
+    <row r="40" spans="1:10" ht="30">
+      <c r="A40" s="39" t="s">
+        <v>56</v>
+      </c>
+      <c r="B40" s="42" t="s">
+        <v>247</v>
+      </c>
       <c r="C40" s="20" t="s">
-        <v>141</v>
-      </c>
-      <c r="D40" s="3"/>
+        <v>100</v>
+      </c>
+      <c r="D40" s="13" t="s">
+        <v>194</v>
+      </c>
       <c r="E40" s="3"/>
       <c r="F40" s="3"/>
       <c r="G40" s="3"/>
       <c r="H40" s="3"/>
-      <c r="I40" s="14"/>
-    </row>
-    <row r="41" spans="1:9" ht="30">
-      <c r="A41" s="45" t="s">
-        <v>56</v>
-      </c>
-      <c r="B41" s="41" t="s">
-        <v>269</v>
-      </c>
+      <c r="I40" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="J40" s="3"/>
+    </row>
+    <row r="41" spans="1:10">
+      <c r="A41" s="43"/>
+      <c r="B41" s="45"/>
       <c r="C41" s="20" t="s">
-        <v>105</v>
-      </c>
-      <c r="D41" s="13" t="s">
-        <v>206</v>
-      </c>
+        <v>135</v>
+      </c>
+      <c r="D41" s="3"/>
       <c r="E41" s="3"/>
       <c r="F41" s="3"/>
       <c r="G41" s="3"/>
       <c r="H41" s="3"/>
-      <c r="I41" s="14" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9">
-      <c r="A42" s="46"/>
-      <c r="B42" s="42"/>
+      <c r="I41" s="14"/>
+      <c r="J41" s="3"/>
+    </row>
+    <row r="42" spans="1:10">
+      <c r="A42" s="43"/>
+      <c r="B42" s="45"/>
       <c r="C42" s="20" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="D42" s="3"/>
       <c r="E42" s="3"/>
@@ -2993,12 +3180,13 @@
       <c r="G42" s="3"/>
       <c r="H42" s="3"/>
       <c r="I42" s="14"/>
-    </row>
-    <row r="43" spans="1:9">
-      <c r="A43" s="46"/>
-      <c r="B43" s="42"/>
+      <c r="J42" s="3"/>
+    </row>
+    <row r="43" spans="1:10">
+      <c r="A43" s="44"/>
+      <c r="B43" s="46"/>
       <c r="C43" s="20" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="D43" s="3"/>
       <c r="E43" s="3"/>
@@ -3006,46 +3194,49 @@
       <c r="G43" s="3"/>
       <c r="H43" s="3"/>
       <c r="I43" s="14"/>
-    </row>
-    <row r="44" spans="1:9">
-      <c r="A44" s="47"/>
-      <c r="B44" s="43"/>
+      <c r="J43" s="3"/>
+    </row>
+    <row r="44" spans="1:10" ht="30">
+      <c r="A44" s="39" t="s">
+        <v>57</v>
+      </c>
+      <c r="B44" s="42" t="s">
+        <v>248</v>
+      </c>
       <c r="C44" s="20" t="s">
-        <v>144</v>
-      </c>
-      <c r="D44" s="3"/>
+        <v>101</v>
+      </c>
+      <c r="D44" s="13" t="s">
+        <v>195</v>
+      </c>
       <c r="E44" s="3"/>
       <c r="F44" s="3"/>
       <c r="G44" s="3"/>
       <c r="H44" s="3"/>
-      <c r="I44" s="14"/>
-    </row>
-    <row r="45" spans="1:9" ht="30">
-      <c r="A45" s="45" t="s">
-        <v>57</v>
-      </c>
-      <c r="B45" s="41" t="s">
-        <v>270</v>
-      </c>
+      <c r="I44" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="J44" s="3"/>
+    </row>
+    <row r="45" spans="1:10">
+      <c r="A45" s="43"/>
+      <c r="B45" s="45"/>
       <c r="C45" s="20" t="s">
-        <v>106</v>
-      </c>
-      <c r="D45" s="13" t="s">
-        <v>207</v>
-      </c>
+        <v>138</v>
+      </c>
+      <c r="D45" s="3"/>
       <c r="E45" s="3"/>
       <c r="F45" s="3"/>
       <c r="G45" s="3"/>
       <c r="H45" s="3"/>
-      <c r="I45" s="14" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9">
-      <c r="A46" s="46"/>
-      <c r="B46" s="42"/>
+      <c r="I45" s="14"/>
+      <c r="J45" s="3"/>
+    </row>
+    <row r="46" spans="1:10">
+      <c r="A46" s="43"/>
+      <c r="B46" s="45"/>
       <c r="C46" s="20" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="D46" s="3"/>
       <c r="E46" s="3"/>
@@ -3053,12 +3244,13 @@
       <c r="G46" s="3"/>
       <c r="H46" s="3"/>
       <c r="I46" s="14"/>
-    </row>
-    <row r="47" spans="1:9">
-      <c r="A47" s="46"/>
-      <c r="B47" s="42"/>
+      <c r="J46" s="3"/>
+    </row>
+    <row r="47" spans="1:10">
+      <c r="A47" s="44"/>
+      <c r="B47" s="46"/>
       <c r="C47" s="20" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="D47" s="3"/>
       <c r="E47" s="3"/>
@@ -3066,46 +3258,49 @@
       <c r="G47" s="3"/>
       <c r="H47" s="3"/>
       <c r="I47" s="14"/>
-    </row>
-    <row r="48" spans="1:9">
-      <c r="A48" s="47"/>
-      <c r="B48" s="43"/>
+      <c r="J47" s="3"/>
+    </row>
+    <row r="48" spans="1:10" ht="39.75" customHeight="1">
+      <c r="A48" s="39" t="s">
+        <v>58</v>
+      </c>
+      <c r="B48" s="42" t="s">
+        <v>249</v>
+      </c>
       <c r="C48" s="20" t="s">
-        <v>147</v>
-      </c>
-      <c r="D48" s="3"/>
+        <v>102</v>
+      </c>
+      <c r="D48" s="13" t="s">
+        <v>196</v>
+      </c>
       <c r="E48" s="3"/>
       <c r="F48" s="3"/>
       <c r="G48" s="3"/>
       <c r="H48" s="3"/>
-      <c r="I48" s="14"/>
-    </row>
-    <row r="49" spans="1:9" ht="45">
-      <c r="A49" s="45" t="s">
-        <v>58</v>
-      </c>
-      <c r="B49" s="41" t="s">
-        <v>271</v>
-      </c>
+      <c r="I48" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="J48" s="3"/>
+    </row>
+    <row r="49" spans="1:10">
+      <c r="A49" s="43"/>
+      <c r="B49" s="45"/>
       <c r="C49" s="20" t="s">
-        <v>107</v>
-      </c>
-      <c r="D49" s="13" t="s">
-        <v>208</v>
-      </c>
+        <v>141</v>
+      </c>
+      <c r="D49" s="3"/>
       <c r="E49" s="3"/>
       <c r="F49" s="3"/>
       <c r="G49" s="3"/>
       <c r="H49" s="3"/>
-      <c r="I49" s="14" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9">
-      <c r="A50" s="46"/>
-      <c r="B50" s="42"/>
+      <c r="I49" s="14"/>
+      <c r="J49" s="3"/>
+    </row>
+    <row r="50" spans="1:10">
+      <c r="A50" s="43"/>
+      <c r="B50" s="45"/>
       <c r="C50" s="20" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="D50" s="3"/>
       <c r="E50" s="3"/>
@@ -3113,12 +3308,13 @@
       <c r="G50" s="3"/>
       <c r="H50" s="3"/>
       <c r="I50" s="14"/>
-    </row>
-    <row r="51" spans="1:9">
-      <c r="A51" s="46"/>
-      <c r="B51" s="42"/>
+      <c r="J50" s="3"/>
+    </row>
+    <row r="51" spans="1:10">
+      <c r="A51" s="44"/>
+      <c r="B51" s="46"/>
       <c r="C51" s="20" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="D51" s="3"/>
       <c r="E51" s="3"/>
@@ -3126,46 +3322,49 @@
       <c r="G51" s="3"/>
       <c r="H51" s="3"/>
       <c r="I51" s="14"/>
-    </row>
-    <row r="52" spans="1:9">
-      <c r="A52" s="47"/>
-      <c r="B52" s="43"/>
+      <c r="J51" s="3"/>
+    </row>
+    <row r="52" spans="1:10">
+      <c r="A52" s="39" t="s">
+        <v>59</v>
+      </c>
+      <c r="B52" s="42" t="s">
+        <v>250</v>
+      </c>
       <c r="C52" s="20" t="s">
-        <v>150</v>
-      </c>
-      <c r="D52" s="3"/>
+        <v>103</v>
+      </c>
+      <c r="D52" s="3" t="s">
+        <v>232</v>
+      </c>
       <c r="E52" s="3"/>
       <c r="F52" s="3"/>
       <c r="G52" s="3"/>
       <c r="H52" s="3"/>
-      <c r="I52" s="14"/>
-    </row>
-    <row r="53" spans="1:9">
-      <c r="A53" s="45" t="s">
-        <v>59</v>
-      </c>
-      <c r="B53" s="41" t="s">
-        <v>272</v>
-      </c>
+      <c r="I52" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="J52" s="3"/>
+    </row>
+    <row r="53" spans="1:10">
+      <c r="A53" s="43"/>
+      <c r="B53" s="45"/>
       <c r="C53" s="20" t="s">
-        <v>108</v>
-      </c>
-      <c r="D53" s="3" t="s">
-        <v>254</v>
-      </c>
+        <v>144</v>
+      </c>
+      <c r="D53" s="3"/>
       <c r="E53" s="3"/>
       <c r="F53" s="3"/>
       <c r="G53" s="3"/>
       <c r="H53" s="3"/>
-      <c r="I53" s="14" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9">
-      <c r="A54" s="46"/>
-      <c r="B54" s="42"/>
+      <c r="I53" s="14"/>
+      <c r="J53" s="3"/>
+    </row>
+    <row r="54" spans="1:10">
+      <c r="A54" s="43"/>
+      <c r="B54" s="45"/>
       <c r="C54" s="20" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="D54" s="3"/>
       <c r="E54" s="3"/>
@@ -3173,12 +3372,13 @@
       <c r="G54" s="3"/>
       <c r="H54" s="3"/>
       <c r="I54" s="14"/>
-    </row>
-    <row r="55" spans="1:9">
-      <c r="A55" s="46"/>
-      <c r="B55" s="42"/>
+      <c r="J54" s="3"/>
+    </row>
+    <row r="55" spans="1:10">
+      <c r="A55" s="44"/>
+      <c r="B55" s="46"/>
       <c r="C55" s="20" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="D55" s="3"/>
       <c r="E55" s="3"/>
@@ -3186,46 +3386,49 @@
       <c r="G55" s="3"/>
       <c r="H55" s="3"/>
       <c r="I55" s="14"/>
-    </row>
-    <row r="56" spans="1:9">
-      <c r="A56" s="47"/>
-      <c r="B56" s="43"/>
+      <c r="J55" s="3"/>
+    </row>
+    <row r="56" spans="1:10">
+      <c r="A56" s="39" t="s">
+        <v>60</v>
+      </c>
+      <c r="B56" s="42" t="s">
+        <v>251</v>
+      </c>
       <c r="C56" s="20" t="s">
-        <v>153</v>
-      </c>
-      <c r="D56" s="3"/>
+        <v>104</v>
+      </c>
+      <c r="D56" s="3" t="s">
+        <v>233</v>
+      </c>
       <c r="E56" s="3"/>
       <c r="F56" s="3"/>
       <c r="G56" s="3"/>
       <c r="H56" s="3"/>
-      <c r="I56" s="14"/>
-    </row>
-    <row r="57" spans="1:9">
-      <c r="A57" s="45" t="s">
-        <v>60</v>
-      </c>
-      <c r="B57" s="41" t="s">
-        <v>273</v>
-      </c>
+      <c r="I56" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="J56" s="3"/>
+    </row>
+    <row r="57" spans="1:10">
+      <c r="A57" s="43"/>
+      <c r="B57" s="45"/>
       <c r="C57" s="20" t="s">
-        <v>109</v>
-      </c>
-      <c r="D57" s="3" t="s">
-        <v>255</v>
-      </c>
+        <v>147</v>
+      </c>
+      <c r="D57" s="3"/>
       <c r="E57" s="3"/>
       <c r="F57" s="3"/>
       <c r="G57" s="3"/>
       <c r="H57" s="3"/>
-      <c r="I57" s="14" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9">
-      <c r="A58" s="46"/>
-      <c r="B58" s="42"/>
+      <c r="I57" s="14"/>
+      <c r="J57" s="3"/>
+    </row>
+    <row r="58" spans="1:10">
+      <c r="A58" s="43"/>
+      <c r="B58" s="45"/>
       <c r="C58" s="20" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="D58" s="3"/>
       <c r="E58" s="3"/>
@@ -3233,12 +3436,13 @@
       <c r="G58" s="3"/>
       <c r="H58" s="3"/>
       <c r="I58" s="14"/>
-    </row>
-    <row r="59" spans="1:9">
-      <c r="A59" s="46"/>
-      <c r="B59" s="42"/>
+      <c r="J58" s="3"/>
+    </row>
+    <row r="59" spans="1:10">
+      <c r="A59" s="44"/>
+      <c r="B59" s="46"/>
       <c r="C59" s="20" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="D59" s="3"/>
       <c r="E59" s="3"/>
@@ -3246,46 +3450,49 @@
       <c r="G59" s="3"/>
       <c r="H59" s="3"/>
       <c r="I59" s="14"/>
-    </row>
-    <row r="60" spans="1:9">
-      <c r="A60" s="47"/>
-      <c r="B60" s="43"/>
+      <c r="J59" s="3"/>
+    </row>
+    <row r="60" spans="1:10">
+      <c r="A60" s="39" t="s">
+        <v>61</v>
+      </c>
+      <c r="B60" s="42" t="s">
+        <v>252</v>
+      </c>
       <c r="C60" s="20" t="s">
-        <v>156</v>
-      </c>
-      <c r="D60" s="3"/>
+        <v>105</v>
+      </c>
+      <c r="D60" s="3" t="s">
+        <v>234</v>
+      </c>
       <c r="E60" s="3"/>
       <c r="F60" s="3"/>
       <c r="G60" s="3"/>
       <c r="H60" s="3"/>
-      <c r="I60" s="14"/>
-    </row>
-    <row r="61" spans="1:9">
-      <c r="A61" s="45" t="s">
-        <v>61</v>
-      </c>
-      <c r="B61" s="41" t="s">
-        <v>274</v>
-      </c>
+      <c r="I60" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="J60" s="3"/>
+    </row>
+    <row r="61" spans="1:10">
+      <c r="A61" s="43"/>
+      <c r="B61" s="45"/>
       <c r="C61" s="20" t="s">
-        <v>110</v>
-      </c>
-      <c r="D61" s="3" t="s">
-        <v>256</v>
-      </c>
+        <v>150</v>
+      </c>
+      <c r="D61" s="3"/>
       <c r="E61" s="3"/>
       <c r="F61" s="3"/>
       <c r="G61" s="3"/>
       <c r="H61" s="3"/>
-      <c r="I61" s="14" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="62" spans="1:9">
-      <c r="A62" s="46"/>
-      <c r="B62" s="42"/>
+      <c r="I61" s="14"/>
+      <c r="J61" s="3"/>
+    </row>
+    <row r="62" spans="1:10">
+      <c r="A62" s="43"/>
+      <c r="B62" s="45"/>
       <c r="C62" s="20" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="D62" s="3"/>
       <c r="E62" s="3"/>
@@ -3293,12 +3500,13 @@
       <c r="G62" s="3"/>
       <c r="H62" s="3"/>
       <c r="I62" s="14"/>
-    </row>
-    <row r="63" spans="1:9">
-      <c r="A63" s="46"/>
-      <c r="B63" s="42"/>
+      <c r="J62" s="3"/>
+    </row>
+    <row r="63" spans="1:10">
+      <c r="A63" s="44"/>
+      <c r="B63" s="46"/>
       <c r="C63" s="20" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="D63" s="3"/>
       <c r="E63" s="3"/>
@@ -3306,46 +3514,49 @@
       <c r="G63" s="3"/>
       <c r="H63" s="3"/>
       <c r="I63" s="14"/>
-    </row>
-    <row r="64" spans="1:9">
-      <c r="A64" s="47"/>
-      <c r="B64" s="43"/>
+      <c r="J63" s="3"/>
+    </row>
+    <row r="64" spans="1:10">
+      <c r="A64" s="39" t="s">
+        <v>62</v>
+      </c>
+      <c r="B64" s="42" t="s">
+        <v>253</v>
+      </c>
       <c r="C64" s="20" t="s">
-        <v>159</v>
-      </c>
-      <c r="D64" s="3"/>
+        <v>106</v>
+      </c>
+      <c r="D64" s="3" t="s">
+        <v>235</v>
+      </c>
       <c r="E64" s="3"/>
       <c r="F64" s="3"/>
       <c r="G64" s="3"/>
       <c r="H64" s="3"/>
-      <c r="I64" s="14"/>
-    </row>
-    <row r="65" spans="1:9">
-      <c r="A65" s="45" t="s">
-        <v>62</v>
-      </c>
-      <c r="B65" s="41" t="s">
-        <v>275</v>
-      </c>
+      <c r="I64" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="J64" s="3"/>
+    </row>
+    <row r="65" spans="1:10">
+      <c r="A65" s="43"/>
+      <c r="B65" s="45"/>
       <c r="C65" s="20" t="s">
-        <v>111</v>
-      </c>
-      <c r="D65" s="3" t="s">
-        <v>257</v>
-      </c>
+        <v>107</v>
+      </c>
+      <c r="D65" s="3"/>
       <c r="E65" s="3"/>
       <c r="F65" s="3"/>
       <c r="G65" s="3"/>
       <c r="H65" s="3"/>
-      <c r="I65" s="14" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="66" spans="1:9">
-      <c r="A66" s="46"/>
-      <c r="B66" s="42"/>
+      <c r="I65" s="14"/>
+      <c r="J65" s="3"/>
+    </row>
+    <row r="66" spans="1:10">
+      <c r="A66" s="43"/>
+      <c r="B66" s="45"/>
       <c r="C66" s="20" t="s">
-        <v>112</v>
+        <v>153</v>
       </c>
       <c r="D66" s="3"/>
       <c r="E66" s="3"/>
@@ -3353,12 +3564,13 @@
       <c r="G66" s="3"/>
       <c r="H66" s="3"/>
       <c r="I66" s="14"/>
-    </row>
-    <row r="67" spans="1:9">
-      <c r="A67" s="46"/>
-      <c r="B67" s="42"/>
+      <c r="J66" s="3"/>
+    </row>
+    <row r="67" spans="1:10">
+      <c r="A67" s="44"/>
+      <c r="B67" s="46"/>
       <c r="C67" s="20" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="D67" s="3"/>
       <c r="E67" s="3"/>
@@ -3366,46 +3578,49 @@
       <c r="G67" s="3"/>
       <c r="H67" s="3"/>
       <c r="I67" s="14"/>
-    </row>
-    <row r="68" spans="1:9">
-      <c r="A68" s="47"/>
-      <c r="B68" s="43"/>
+      <c r="J67" s="3"/>
+    </row>
+    <row r="68" spans="1:10">
+      <c r="A68" s="39" t="s">
+        <v>63</v>
+      </c>
+      <c r="B68" s="42" t="s">
+        <v>254</v>
+      </c>
       <c r="C68" s="20" t="s">
-        <v>161</v>
-      </c>
-      <c r="D68" s="3"/>
+        <v>108</v>
+      </c>
+      <c r="D68" s="3" t="s">
+        <v>236</v>
+      </c>
       <c r="E68" s="3"/>
       <c r="F68" s="3"/>
       <c r="G68" s="3"/>
       <c r="H68" s="3"/>
-      <c r="I68" s="14"/>
-    </row>
-    <row r="69" spans="1:9">
-      <c r="A69" s="45" t="s">
-        <v>63</v>
-      </c>
-      <c r="B69" s="41" t="s">
-        <v>276</v>
-      </c>
+      <c r="I68" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="J68" s="3"/>
+    </row>
+    <row r="69" spans="1:10">
+      <c r="A69" s="43"/>
+      <c r="B69" s="45"/>
       <c r="C69" s="20" t="s">
-        <v>113</v>
-      </c>
-      <c r="D69" s="3" t="s">
-        <v>258</v>
-      </c>
+        <v>155</v>
+      </c>
+      <c r="D69" s="3"/>
       <c r="E69" s="3"/>
       <c r="F69" s="3"/>
       <c r="G69" s="3"/>
       <c r="H69" s="3"/>
-      <c r="I69" s="14" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="70" spans="1:9">
-      <c r="A70" s="46"/>
-      <c r="B70" s="42"/>
+      <c r="I69" s="14"/>
+      <c r="J69" s="3"/>
+    </row>
+    <row r="70" spans="1:10">
+      <c r="A70" s="43"/>
+      <c r="B70" s="45"/>
       <c r="C70" s="20" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="D70" s="3"/>
       <c r="E70" s="3"/>
@@ -3413,12 +3628,13 @@
       <c r="G70" s="3"/>
       <c r="H70" s="3"/>
       <c r="I70" s="14"/>
-    </row>
-    <row r="71" spans="1:9">
-      <c r="A71" s="46"/>
-      <c r="B71" s="42"/>
+      <c r="J70" s="3"/>
+    </row>
+    <row r="71" spans="1:10">
+      <c r="A71" s="44"/>
+      <c r="B71" s="46"/>
       <c r="C71" s="20" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="D71" s="3"/>
       <c r="E71" s="3"/>
@@ -3426,46 +3642,49 @@
       <c r="G71" s="3"/>
       <c r="H71" s="3"/>
       <c r="I71" s="14"/>
-    </row>
-    <row r="72" spans="1:9">
-      <c r="A72" s="47"/>
-      <c r="B72" s="43"/>
+      <c r="J71" s="3"/>
+    </row>
+    <row r="72" spans="1:10">
+      <c r="A72" s="39" t="s">
+        <v>64</v>
+      </c>
+      <c r="B72" s="42" t="s">
+        <v>255</v>
+      </c>
       <c r="C72" s="20" t="s">
-        <v>164</v>
-      </c>
-      <c r="D72" s="3"/>
+        <v>109</v>
+      </c>
+      <c r="D72" s="3" t="s">
+        <v>239</v>
+      </c>
       <c r="E72" s="3"/>
       <c r="F72" s="3"/>
       <c r="G72" s="3"/>
       <c r="H72" s="3"/>
-      <c r="I72" s="14"/>
-    </row>
-    <row r="73" spans="1:9">
-      <c r="A73" s="45" t="s">
-        <v>64</v>
-      </c>
-      <c r="B73" s="41" t="s">
-        <v>277</v>
-      </c>
+      <c r="I72" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="J72" s="3"/>
+    </row>
+    <row r="73" spans="1:10">
+      <c r="A73" s="43"/>
+      <c r="B73" s="45"/>
       <c r="C73" s="20" t="s">
-        <v>114</v>
-      </c>
-      <c r="D73" s="3" t="s">
-        <v>261</v>
-      </c>
+        <v>158</v>
+      </c>
+      <c r="D73" s="3"/>
       <c r="E73" s="3"/>
       <c r="F73" s="3"/>
       <c r="G73" s="3"/>
       <c r="H73" s="3"/>
-      <c r="I73" s="14" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="74" spans="1:9">
-      <c r="A74" s="46"/>
-      <c r="B74" s="42"/>
+      <c r="I73" s="14"/>
+      <c r="J73" s="3"/>
+    </row>
+    <row r="74" spans="1:10">
+      <c r="A74" s="43"/>
+      <c r="B74" s="45"/>
       <c r="C74" s="20" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="D74" s="3"/>
       <c r="E74" s="3"/>
@@ -3473,12 +3692,13 @@
       <c r="G74" s="3"/>
       <c r="H74" s="3"/>
       <c r="I74" s="14"/>
-    </row>
-    <row r="75" spans="1:9">
-      <c r="A75" s="46"/>
-      <c r="B75" s="42"/>
+      <c r="J74" s="3"/>
+    </row>
+    <row r="75" spans="1:10">
+      <c r="A75" s="44"/>
+      <c r="B75" s="46"/>
       <c r="C75" s="20" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="D75" s="3"/>
       <c r="E75" s="3"/>
@@ -3486,46 +3706,49 @@
       <c r="G75" s="3"/>
       <c r="H75" s="3"/>
       <c r="I75" s="14"/>
-    </row>
-    <row r="76" spans="1:9">
-      <c r="A76" s="47"/>
-      <c r="B76" s="43"/>
+      <c r="J75" s="3"/>
+    </row>
+    <row r="76" spans="1:10">
+      <c r="A76" s="39" t="s">
+        <v>65</v>
+      </c>
+      <c r="B76" s="42" t="s">
+        <v>256</v>
+      </c>
       <c r="C76" s="20" t="s">
-        <v>167</v>
-      </c>
-      <c r="D76" s="3"/>
+        <v>110</v>
+      </c>
+      <c r="D76" s="3" t="s">
+        <v>240</v>
+      </c>
       <c r="E76" s="3"/>
       <c r="F76" s="3"/>
       <c r="G76" s="3"/>
       <c r="H76" s="3"/>
-      <c r="I76" s="14"/>
-    </row>
-    <row r="77" spans="1:9">
-      <c r="A77" s="45" t="s">
-        <v>65</v>
-      </c>
-      <c r="B77" s="41" t="s">
-        <v>278</v>
-      </c>
+      <c r="I76" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="J76" s="3"/>
+    </row>
+    <row r="77" spans="1:10">
+      <c r="A77" s="43"/>
+      <c r="B77" s="45"/>
       <c r="C77" s="20" t="s">
-        <v>115</v>
-      </c>
-      <c r="D77" s="3" t="s">
-        <v>262</v>
-      </c>
+        <v>111</v>
+      </c>
+      <c r="D77" s="3"/>
       <c r="E77" s="3"/>
       <c r="F77" s="3"/>
       <c r="G77" s="3"/>
       <c r="H77" s="3"/>
-      <c r="I77" s="14" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="78" spans="1:9">
-      <c r="A78" s="46"/>
-      <c r="B78" s="42"/>
+      <c r="I77" s="14"/>
+      <c r="J77" s="3"/>
+    </row>
+    <row r="78" spans="1:10">
+      <c r="A78" s="43"/>
+      <c r="B78" s="45"/>
       <c r="C78" s="20" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="D78" s="3"/>
       <c r="E78" s="3"/>
@@ -3533,12 +3756,13 @@
       <c r="G78" s="3"/>
       <c r="H78" s="3"/>
       <c r="I78" s="14"/>
-    </row>
-    <row r="79" spans="1:9">
-      <c r="A79" s="46"/>
-      <c r="B79" s="42"/>
+      <c r="J78" s="3"/>
+    </row>
+    <row r="79" spans="1:10">
+      <c r="A79" s="44"/>
+      <c r="B79" s="46"/>
       <c r="C79" s="20" t="s">
-        <v>117</v>
+        <v>161</v>
       </c>
       <c r="D79" s="3"/>
       <c r="E79" s="3"/>
@@ -3546,46 +3770,49 @@
       <c r="G79" s="3"/>
       <c r="H79" s="3"/>
       <c r="I79" s="14"/>
-    </row>
-    <row r="80" spans="1:9">
-      <c r="A80" s="47"/>
-      <c r="B80" s="43"/>
+      <c r="J79" s="3"/>
+    </row>
+    <row r="80" spans="1:10">
+      <c r="A80" s="39" t="s">
+        <v>66</v>
+      </c>
+      <c r="B80" s="42" t="s">
+        <v>257</v>
+      </c>
       <c r="C80" s="20" t="s">
-        <v>168</v>
-      </c>
-      <c r="D80" s="3"/>
+        <v>113</v>
+      </c>
+      <c r="D80" s="3" t="s">
+        <v>241</v>
+      </c>
       <c r="E80" s="3"/>
       <c r="F80" s="3"/>
       <c r="G80" s="3"/>
       <c r="H80" s="3"/>
-      <c r="I80" s="14"/>
-    </row>
-    <row r="81" spans="1:9">
-      <c r="A81" s="45" t="s">
-        <v>66</v>
-      </c>
-      <c r="B81" s="41" t="s">
-        <v>279</v>
-      </c>
+      <c r="I80" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="J80" s="3"/>
+    </row>
+    <row r="81" spans="1:10">
+      <c r="A81" s="43"/>
+      <c r="B81" s="45"/>
       <c r="C81" s="20" t="s">
-        <v>118</v>
-      </c>
-      <c r="D81" s="3" t="s">
-        <v>263</v>
-      </c>
+        <v>162</v>
+      </c>
+      <c r="D81" s="3"/>
       <c r="E81" s="3"/>
       <c r="F81" s="3"/>
       <c r="G81" s="3"/>
       <c r="H81" s="3"/>
-      <c r="I81" s="14" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="82" spans="1:9">
-      <c r="A82" s="46"/>
-      <c r="B82" s="42"/>
+      <c r="I81" s="14"/>
+      <c r="J81" s="3"/>
+    </row>
+    <row r="82" spans="1:10">
+      <c r="A82" s="43"/>
+      <c r="B82" s="45"/>
       <c r="C82" s="20" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="D82" s="3"/>
       <c r="E82" s="3"/>
@@ -3593,12 +3820,13 @@
       <c r="G82" s="3"/>
       <c r="H82" s="3"/>
       <c r="I82" s="14"/>
-    </row>
-    <row r="83" spans="1:9">
-      <c r="A83" s="46"/>
-      <c r="B83" s="42"/>
+      <c r="J82" s="3"/>
+    </row>
+    <row r="83" spans="1:10">
+      <c r="A83" s="44"/>
+      <c r="B83" s="46"/>
       <c r="C83" s="20" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="D83" s="3"/>
       <c r="E83" s="3"/>
@@ -3606,46 +3834,49 @@
       <c r="G83" s="3"/>
       <c r="H83" s="3"/>
       <c r="I83" s="14"/>
-    </row>
-    <row r="84" spans="1:9">
-      <c r="A84" s="47"/>
-      <c r="B84" s="43"/>
+      <c r="J83" s="3"/>
+    </row>
+    <row r="84" spans="1:10">
+      <c r="A84" s="39" t="s">
+        <v>67</v>
+      </c>
+      <c r="B84" s="42" t="s">
+        <v>258</v>
+      </c>
       <c r="C84" s="20" t="s">
-        <v>171</v>
-      </c>
-      <c r="D84" s="3"/>
+        <v>114</v>
+      </c>
+      <c r="D84" s="3" t="s">
+        <v>242</v>
+      </c>
       <c r="E84" s="3"/>
       <c r="F84" s="3"/>
       <c r="G84" s="3"/>
       <c r="H84" s="3"/>
-      <c r="I84" s="14"/>
-    </row>
-    <row r="85" spans="1:9">
-      <c r="A85" s="45" t="s">
-        <v>67</v>
-      </c>
-      <c r="B85" s="41" t="s">
-        <v>280</v>
-      </c>
+      <c r="I84" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="J84" s="3"/>
+    </row>
+    <row r="85" spans="1:10">
+      <c r="A85" s="43"/>
+      <c r="B85" s="45"/>
       <c r="C85" s="20" t="s">
-        <v>119</v>
-      </c>
-      <c r="D85" s="3" t="s">
-        <v>264</v>
-      </c>
+        <v>165</v>
+      </c>
+      <c r="D85" s="3"/>
       <c r="E85" s="3"/>
       <c r="F85" s="3"/>
       <c r="G85" s="3"/>
       <c r="H85" s="3"/>
-      <c r="I85" s="14" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="86" spans="1:9">
-      <c r="A86" s="46"/>
-      <c r="B86" s="42"/>
+      <c r="I85" s="14"/>
+      <c r="J85" s="3"/>
+    </row>
+    <row r="86" spans="1:10">
+      <c r="A86" s="43"/>
+      <c r="B86" s="45"/>
       <c r="C86" s="20" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="D86" s="3"/>
       <c r="E86" s="3"/>
@@ -3653,12 +3884,13 @@
       <c r="G86" s="3"/>
       <c r="H86" s="3"/>
       <c r="I86" s="14"/>
-    </row>
-    <row r="87" spans="1:9">
-      <c r="A87" s="46"/>
-      <c r="B87" s="42"/>
+      <c r="J86" s="3"/>
+    </row>
+    <row r="87" spans="1:10">
+      <c r="A87" s="44"/>
+      <c r="B87" s="46"/>
       <c r="C87" s="20" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="D87" s="3"/>
       <c r="E87" s="3"/>
@@ -3666,46 +3898,49 @@
       <c r="G87" s="3"/>
       <c r="H87" s="3"/>
       <c r="I87" s="14"/>
-    </row>
-    <row r="88" spans="1:9">
-      <c r="A88" s="47"/>
-      <c r="B88" s="43"/>
+      <c r="J87" s="3"/>
+    </row>
+    <row r="88" spans="1:10">
+      <c r="A88" s="39" t="s">
+        <v>68</v>
+      </c>
+      <c r="B88" s="42" t="s">
+        <v>259</v>
+      </c>
       <c r="C88" s="20" t="s">
-        <v>174</v>
-      </c>
-      <c r="D88" s="3"/>
+        <v>115</v>
+      </c>
+      <c r="D88" s="3" t="s">
+        <v>243</v>
+      </c>
       <c r="E88" s="3"/>
       <c r="F88" s="3"/>
       <c r="G88" s="3"/>
       <c r="H88" s="3"/>
-      <c r="I88" s="14"/>
-    </row>
-    <row r="89" spans="1:9">
-      <c r="A89" s="45" t="s">
-        <v>68</v>
-      </c>
-      <c r="B89" s="41" t="s">
-        <v>281</v>
-      </c>
+      <c r="I88" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="J88" s="3"/>
+    </row>
+    <row r="89" spans="1:10">
+      <c r="A89" s="43"/>
+      <c r="B89" s="45"/>
       <c r="C89" s="20" t="s">
-        <v>120</v>
-      </c>
-      <c r="D89" s="3" t="s">
-        <v>265</v>
-      </c>
+        <v>168</v>
+      </c>
+      <c r="D89" s="3"/>
       <c r="E89" s="3"/>
       <c r="F89" s="3"/>
       <c r="G89" s="3"/>
       <c r="H89" s="3"/>
-      <c r="I89" s="14" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="90" spans="1:9">
-      <c r="A90" s="46"/>
-      <c r="B90" s="42"/>
+      <c r="I89" s="14"/>
+      <c r="J89" s="3"/>
+    </row>
+    <row r="90" spans="1:10">
+      <c r="A90" s="43"/>
+      <c r="B90" s="45"/>
       <c r="C90" s="20" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="D90" s="3"/>
       <c r="E90" s="3"/>
@@ -3713,12 +3948,13 @@
       <c r="G90" s="3"/>
       <c r="H90" s="3"/>
       <c r="I90" s="14"/>
-    </row>
-    <row r="91" spans="1:9">
-      <c r="A91" s="46"/>
-      <c r="B91" s="42"/>
+      <c r="J90" s="3"/>
+    </row>
+    <row r="91" spans="1:10">
+      <c r="A91" s="44"/>
+      <c r="B91" s="46"/>
       <c r="C91" s="20" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="D91" s="3"/>
       <c r="E91" s="3"/>
@@ -3726,46 +3962,49 @@
       <c r="G91" s="3"/>
       <c r="H91" s="3"/>
       <c r="I91" s="14"/>
-    </row>
-    <row r="92" spans="1:9">
-      <c r="A92" s="47"/>
-      <c r="B92" s="43"/>
+      <c r="J91" s="3"/>
+    </row>
+    <row r="92" spans="1:10">
+      <c r="A92" s="39" t="s">
+        <v>69</v>
+      </c>
+      <c r="B92" s="42" t="s">
+        <v>260</v>
+      </c>
       <c r="C92" s="20" t="s">
-        <v>177</v>
-      </c>
-      <c r="D92" s="3"/>
+        <v>116</v>
+      </c>
+      <c r="D92" s="3" t="s">
+        <v>244</v>
+      </c>
       <c r="E92" s="3"/>
       <c r="F92" s="3"/>
       <c r="G92" s="3"/>
       <c r="H92" s="3"/>
-      <c r="I92" s="14"/>
-    </row>
-    <row r="93" spans="1:9">
-      <c r="A93" s="45" t="s">
-        <v>69</v>
-      </c>
-      <c r="B93" s="41" t="s">
-        <v>282</v>
-      </c>
+      <c r="I92" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="J92" s="3"/>
+    </row>
+    <row r="93" spans="1:10">
+      <c r="A93" s="43"/>
+      <c r="B93" s="45"/>
       <c r="C93" s="20" t="s">
-        <v>121</v>
-      </c>
-      <c r="D93" s="3" t="s">
-        <v>266</v>
-      </c>
+        <v>171</v>
+      </c>
+      <c r="D93" s="3"/>
       <c r="E93" s="3"/>
       <c r="F93" s="3"/>
       <c r="G93" s="3"/>
       <c r="H93" s="3"/>
-      <c r="I93" s="14" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="94" spans="1:9">
-      <c r="A94" s="46"/>
-      <c r="B94" s="42"/>
+      <c r="I93" s="14"/>
+      <c r="J93" s="3"/>
+    </row>
+    <row r="94" spans="1:10">
+      <c r="A94" s="43"/>
+      <c r="B94" s="45"/>
       <c r="C94" s="20" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="D94" s="3"/>
       <c r="E94" s="3"/>
@@ -3773,12 +4012,13 @@
       <c r="G94" s="3"/>
       <c r="H94" s="3"/>
       <c r="I94" s="14"/>
-    </row>
-    <row r="95" spans="1:9">
-      <c r="A95" s="46"/>
-      <c r="B95" s="42"/>
+      <c r="J94" s="3"/>
+    </row>
+    <row r="95" spans="1:10">
+      <c r="A95" s="44"/>
+      <c r="B95" s="46"/>
       <c r="C95" s="20" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="D95" s="3"/>
       <c r="E95" s="3"/>
@@ -3786,46 +4026,49 @@
       <c r="G95" s="3"/>
       <c r="H95" s="3"/>
       <c r="I95" s="14"/>
-    </row>
-    <row r="96" spans="1:9">
-      <c r="A96" s="47"/>
-      <c r="B96" s="43"/>
+      <c r="J95" s="3"/>
+    </row>
+    <row r="96" spans="1:10">
+      <c r="A96" s="39" t="s">
+        <v>70</v>
+      </c>
+      <c r="B96" s="42" t="s">
+        <v>261</v>
+      </c>
       <c r="C96" s="20" t="s">
-        <v>180</v>
-      </c>
-      <c r="D96" s="3"/>
+        <v>117</v>
+      </c>
+      <c r="D96" s="3" t="s">
+        <v>235</v>
+      </c>
       <c r="E96" s="3"/>
       <c r="F96" s="3"/>
       <c r="G96" s="3"/>
       <c r="H96" s="3"/>
-      <c r="I96" s="14"/>
-    </row>
-    <row r="97" spans="1:9">
-      <c r="A97" s="45" t="s">
-        <v>70</v>
-      </c>
-      <c r="B97" s="41" t="s">
-        <v>283</v>
-      </c>
+      <c r="I96" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="J96" s="3"/>
+    </row>
+    <row r="97" spans="1:10">
+      <c r="A97" s="43"/>
+      <c r="B97" s="45"/>
       <c r="C97" s="20" t="s">
-        <v>122</v>
-      </c>
-      <c r="D97" s="3" t="s">
-        <v>257</v>
-      </c>
+        <v>174</v>
+      </c>
+      <c r="D97" s="3"/>
       <c r="E97" s="3"/>
       <c r="F97" s="3"/>
       <c r="G97" s="3"/>
       <c r="H97" s="3"/>
-      <c r="I97" s="14" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="98" spans="1:9">
-      <c r="A98" s="46"/>
-      <c r="B98" s="42"/>
+      <c r="I97" s="14"/>
+      <c r="J97" s="3"/>
+    </row>
+    <row r="98" spans="1:10">
+      <c r="A98" s="43"/>
+      <c r="B98" s="45"/>
       <c r="C98" s="20" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="D98" s="3"/>
       <c r="E98" s="3"/>
@@ -3833,12 +4076,13 @@
       <c r="G98" s="3"/>
       <c r="H98" s="3"/>
       <c r="I98" s="14"/>
-    </row>
-    <row r="99" spans="1:9">
-      <c r="A99" s="46"/>
-      <c r="B99" s="42"/>
+      <c r="J98" s="3"/>
+    </row>
+    <row r="99" spans="1:10">
+      <c r="A99" s="44"/>
+      <c r="B99" s="46"/>
       <c r="C99" s="20" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="D99" s="3"/>
       <c r="E99" s="3"/>
@@ -3846,59 +4090,63 @@
       <c r="G99" s="3"/>
       <c r="H99" s="3"/>
       <c r="I99" s="14"/>
-    </row>
-    <row r="100" spans="1:9">
-      <c r="A100" s="47"/>
-      <c r="B100" s="43"/>
+      <c r="J99" s="3"/>
+    </row>
+    <row r="100" spans="1:10">
+      <c r="A100" s="39" t="s">
+        <v>71</v>
+      </c>
+      <c r="B100" s="42" t="s">
+        <v>262</v>
+      </c>
       <c r="C100" s="20" t="s">
-        <v>183</v>
-      </c>
-      <c r="D100" s="3"/>
+        <v>118</v>
+      </c>
+      <c r="D100" s="3" t="s">
+        <v>245</v>
+      </c>
       <c r="E100" s="3"/>
       <c r="F100" s="3"/>
       <c r="G100" s="3"/>
       <c r="H100" s="3"/>
       <c r="I100" s="14"/>
-    </row>
-    <row r="101" spans="1:9">
-      <c r="A101" s="45" t="s">
-        <v>71</v>
-      </c>
-      <c r="B101" s="41" t="s">
-        <v>284</v>
-      </c>
+      <c r="J100" s="3"/>
+    </row>
+    <row r="101" spans="1:10">
+      <c r="A101" s="40"/>
+      <c r="B101" s="40"/>
       <c r="C101" s="20" t="s">
-        <v>123</v>
-      </c>
-      <c r="D101" s="3" t="s">
-        <v>267</v>
-      </c>
+        <v>177</v>
+      </c>
+      <c r="D101" s="3"/>
       <c r="E101" s="3"/>
       <c r="F101" s="3"/>
       <c r="G101" s="3"/>
       <c r="H101" s="3"/>
-      <c r="I101" s="14"/>
-    </row>
-    <row r="102" spans="1:9">
-      <c r="A102" s="48"/>
-      <c r="B102" s="48"/>
+      <c r="I101" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="J101" s="3"/>
+    </row>
+    <row r="102" spans="1:10">
+      <c r="A102" s="40"/>
+      <c r="B102" s="40"/>
       <c r="C102" s="20" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="D102" s="3"/>
       <c r="E102" s="3"/>
       <c r="F102" s="3"/>
       <c r="G102" s="3"/>
       <c r="H102" s="3"/>
-      <c r="I102" s="14" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="103" spans="1:9">
-      <c r="A103" s="48"/>
-      <c r="B103" s="48"/>
+      <c r="I102" s="14"/>
+      <c r="J102" s="3"/>
+    </row>
+    <row r="103" spans="1:10">
+      <c r="A103" s="41"/>
+      <c r="B103" s="41"/>
       <c r="C103" s="20" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="D103" s="3"/>
       <c r="E103" s="3"/>
@@ -3906,124 +4154,232 @@
       <c r="G103" s="3"/>
       <c r="H103" s="3"/>
       <c r="I103" s="14"/>
-    </row>
-    <row r="104" spans="1:9">
-      <c r="A104" s="49"/>
-      <c r="B104" s="49"/>
-      <c r="C104" s="20" t="s">
-        <v>186</v>
-      </c>
-      <c r="D104" s="3"/>
+      <c r="J103" s="3"/>
+    </row>
+    <row r="104" spans="1:10">
+      <c r="A104" s="52" t="s">
+        <v>266</v>
+      </c>
+      <c r="B104" s="55" t="s">
+        <v>285</v>
+      </c>
+      <c r="C104" s="3" t="s">
+        <v>267</v>
+      </c>
+      <c r="D104" s="3" t="s">
+        <v>278</v>
+      </c>
       <c r="E104" s="3"/>
       <c r="F104" s="3"/>
-      <c r="G104" s="3"/>
-      <c r="H104" s="3"/>
-      <c r="I104" s="14"/>
-    </row>
-    <row r="107" spans="1:9">
-      <c r="H107" s="15" t="s">
+      <c r="G104" s="3" t="s">
+        <v>270</v>
+      </c>
+      <c r="H104" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="I104" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="J104" s="3"/>
+    </row>
+    <row r="105" spans="1:10">
+      <c r="A105" s="53"/>
+      <c r="B105" s="53"/>
+      <c r="C105" s="3" t="s">
+        <v>268</v>
+      </c>
+      <c r="D105" s="3" t="s">
+        <v>279</v>
+      </c>
+      <c r="E105" s="3"/>
+      <c r="F105" s="3"/>
+      <c r="G105" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="H105" s="3" t="s">
+        <v>273</v>
+      </c>
+      <c r="I105" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="J105" s="3"/>
+    </row>
+    <row r="106" spans="1:10" ht="50.25" customHeight="1">
+      <c r="A106" s="53"/>
+      <c r="B106" s="53"/>
+      <c r="C106" s="52" t="s">
+        <v>269</v>
+      </c>
+      <c r="D106" s="52" t="s">
+        <v>277</v>
+      </c>
+      <c r="E106" s="51"/>
+      <c r="F106" s="51"/>
+      <c r="G106" s="13" t="s">
+        <v>280</v>
+      </c>
+      <c r="H106" s="3" t="s">
+        <v>275</v>
+      </c>
+      <c r="I106" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="J106" s="3"/>
+    </row>
+    <row r="107" spans="1:10" ht="71.25" customHeight="1">
+      <c r="A107" s="53"/>
+      <c r="B107" s="53"/>
+      <c r="C107" s="54"/>
+      <c r="D107" s="54"/>
+      <c r="E107" s="41"/>
+      <c r="F107" s="41"/>
+      <c r="G107" s="3" t="s">
+        <v>276</v>
+      </c>
+      <c r="H107" s="13" t="s">
+        <v>281</v>
+      </c>
+      <c r="I107" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="J107" s="3" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="108" spans="1:10" ht="63.75" customHeight="1">
+      <c r="A108" s="54"/>
+      <c r="B108" s="54"/>
+      <c r="C108" s="24" t="s">
+        <v>274</v>
+      </c>
+      <c r="D108" s="24" t="s">
+        <v>282</v>
+      </c>
+      <c r="E108" s="50"/>
+      <c r="F108" s="50"/>
+      <c r="G108" s="13" t="s">
+        <v>283</v>
+      </c>
+      <c r="H108" s="13" t="s">
+        <v>284</v>
+      </c>
+      <c r="I108" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="J108" s="13" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="110" spans="1:10">
+      <c r="H110" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="I107" s="16">
+      <c r="I110" s="16" t="e">
         <f>IF(I3=P1,1,0)+IF(I4=P1,1,0)+IF(I5=P1,1,0)+IF(I6=P1,1,0)+
 IF(I7=P1,1,0)+IF(I8=P1,1,0)+IF(I9=P1,1,0)+IF(I10=P1,1,0)+
-IF(I11=P1,1,0)+IF(I12=P1,1,0)+IF(I13=P1,1,0)+IF(I14=P1,1,0)+
-IF(I15=P1,1,0)+IF(I16=P1,1,0)+IF(I17=P1,1,0)+IF(I18=P1,1,0)+
-IF(I19=P1,1,0)+IF(I20=P1,1,0)+IF(I21=P1,1,0)+IF(I22=P1,1,0)+
-IF(I23=P1,1,0)+IF(I24=P1,1,0)+IF(I25=P1,1,0)+IF(I26=P1,1,0)+
-IF(I27=P1,1,0)+IF(I28=P1,1,0)+IF(I29=P1,1,0)+IF(I30=P1,1,0)+
-IF(I31=P1,1,0)+IF(I32=P1,1,0)+IF(I33=P1,1,0)+IF(I34=P1,1,0)+
-IF(I35=P1,1,0)+IF(I36=P1,1,0)+IF(I37=P1,1,0)+IF(I38=P1,1,0)+
-IF(I39=P1,1,0)+IF(I40=P1,1,0)+IF(I41=P1,1,0)+IF(I42=P1,1,0)+
-IF(I43=P1,1,0)+IF(I44=P1,1,0)+IF(I45=P1,1,0)+IF(I46=P1,1,0)+
-IF(I47=P1,1,0)+IF(I48=P1,1,0)+IF(I49=P1,1,0)+IF(I50=P1,1,0)+
-IF(I51=P1,1,0)+IF(I52=P1,1,0)+IF(I53=P1,1,0)+IF(I54=P1,1,0)+
-IF(I55=P1,1,0)+IF(I56=P1,1,0)+IF(I57=P1,1,0)+IF(I58=P1,1,0)+
-IF(I59=P1,1,0)+IF(I60=P1,1,0)+IF(I61=P1,1,0)+IF(I62=P1,1,0)+
-IF(I63=P1,1,0)+IF(I64=P1,1,0)+IF(I65=P1,1,0)+IF(I66=P1,1,0)+
-IF(I67=P1,1,0)+IF(I68=P1,1,0)+IF(I69=P1,1,0)+IF(I70=P1,1,0)+
-IF(I71=P1,1,0)+IF(I72=P1,1,0)+IF(I73=P1,1,0)+IF(I74=P1,1,0)+
-IF(I75=P1,1,0)+IF(I76=P1,1,0)+IF(I77=P1,1,0)+IF(I78=P1,1,0)+
-IF(I79=P1,1,0)+IF(I80=P1,1,0)+IF(I81=P1,1,0)+IF(I82=P1,1,0)+
-IF(I83=P1,1,0)+IF(I84=P1,1,0)+IF(I85=P1,1,0)+IF(I86=P1,1,0)+
-IF(I87=P1,1,0)+IF(I88=P1,1,0)+IF(I89=P1,1,0)+IF(I90=P1,1,0)+
-IF(I91=P1,1,0)+IF(I92=P1,1,0)+IF(I93=P1,1,0)+IF(I94=P1,1,0)+
-IF(I95=P1,1,0)+IF(I96=P1,1,0)+IF(I97=P1,1,0)+IF(I98=P1,1,0)+
-IF(I99=P1,1,0)+IF(I100=P1,1,0)+IF(I101=P1,1,0)+IF(I102=P1,1,0)+
-+IF(I103=P1,1,0)+IF(I104=P1,1,0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="108" spans="1:9">
-      <c r="H108" s="15" t="s">
+IF(I12=P1,1,0)+IF(I13=P1,1,0)+IF(I14=P1,1,0)+IF(I15=P1,1,0)+
+IF(I16=P1,1,0)+IF(I17=P1,1,0)+IF(I18=P1,1,0)+IF(I19=P1,1,0)+
+IF(I20=P1,1,0)+IF(I21=P1,1,0)+IF(I22=P1,1,0)+IF(I23=P1,1,0)+
+IF(I24=P1,1,0)+IF(I25=P1,1,0)+IF(I26=P1,1,0)+IF(I27=P1,1,0)+
+IF(I28=P1,1,0)+IF(I29=P1,1,0)+IF(#REF!=P1,1,0)+IF(#REF!=P1,1,0)+
+IF(#REF!=P1,1,0)+IF(#REF!=P1,1,0)+IF(I32=P1,1,0)+IF(I33=P1,1,0)+
+IF(I34=P1,1,0)+IF(I35=P1,1,0)+IF(I36=P1,1,0)+IF(I37=P1,1,0)+
+IF(I38=P1,1,0)+IF(I39=P1,1,0)+IF(I40=P1,1,0)+IF(I41=P1,1,0)+
+IF(I42=P1,1,0)+IF(I43=P1,1,0)+IF(I44=P1,1,0)+IF(I45=P1,1,0)+
+IF(I46=P1,1,0)+IF(I47=P1,1,0)+IF(I48=P1,1,0)+IF(I49=P1,1,0)+
+IF(I50=P1,1,0)+IF(I51=P1,1,0)+IF(I52=P1,1,0)+IF(I53=P1,1,0)+
+IF(I54=P1,1,0)+IF(I55=P1,1,0)+IF(I56=P1,1,0)+IF(I57=P1,1,0)+
+IF(I58=P1,1,0)+IF(I59=P1,1,0)+IF(I60=P1,1,0)+IF(I61=P1,1,0)+
+IF(I62=P1,1,0)+IF(I63=P1,1,0)+IF(I64=P1,1,0)+IF(I65=P1,1,0)+
+IF(I66=P1,1,0)+IF(I67=P1,1,0)+IF(I68=P1,1,0)+IF(I69=P1,1,0)+
+IF(I70=P1,1,0)+IF(I71=P1,1,0)+IF(I72=P1,1,0)+IF(I73=P1,1,0)+
+IF(I74=P1,1,0)+IF(I75=P1,1,0)+IF(I76=P1,1,0)+IF(I77=P1,1,0)+
+IF(I78=P1,1,0)+IF(I79=P1,1,0)+IF(I80=P1,1,0)+IF(I81=P1,1,0)+
+IF(I82=P1,1,0)+IF(I83=P1,1,0)+IF(I84=P1,1,0)+IF(I85=P1,1,0)+
+IF(I86=P1,1,0)+IF(I87=P1,1,0)+IF(I88=P1,1,0)+IF(I89=P1,1,0)+
+IF(I90=P1,1,0)+IF(I91=P1,1,0)+IF(I92=P1,1,0)+IF(I93=P1,1,0)+
+IF(I94=P1,1,0)+IF(I95=P1,1,0)+IF(I96=P1,1,0)+IF(I97=P1,1,0)+
+IF(I98=P1,1,0)+IF(I99=P1,1,0)+IF(I100=P1,1,0)+IF(I101=P1,1,0)+
++IF(I102=P1,1,0)+IF(I103=P1,1,0)</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="111" spans="1:10">
+      <c r="H111" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="I108" s="17">
-        <f>IF(I3=Q1,1,0)+IF(I7=Q1,1,0)+IF(I11=Q1,1,0)+IF(I17=Q1,1,0)+IF(I21=Q1,1,0)+IF(I25=Q1,1,0)+IF(I29=Q1,1,0)+IF(I33=Q1,1,0)+IF(I37=Q1,1,0)+IF(I41=Q1,1,0)+IF(I45=Q1,1,0)+IF(I49=Q1,1,0)+IF(I53=Q1,1,0)+IF(I57=Q1,1,0)+IF(I61=Q1,1,0)+IF(I65=Q1,1,0)+IF(I69=Q1,1,0)+IF(I73=Q1,1,0)+IF(I77=Q1,1,0)+IF(I81=Q1,1,0)+IF(I85=Q1,1,0)+IF(I89=Q1,1,0)+IF(I93=Q1,1,0)+IF(I97=Q1,1,0)+IF(I101=Q1,1,0)+IF(I102=Q1,1,0)+IF(I103=Q1,1,0)+IF(I104=Q1,1,0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="109" spans="1:9">
-      <c r="H109" s="15" t="s">
+      <c r="I111" s="17" t="e">
+        <f>IF(I3=Q1,1,0)+IF(I7=Q1,1,0)+IF(I12=Q1,1,0)+IF(I18=Q1,1,0)+IF(I22=Q1,1,0)+IF(I26=Q1,1,0)+IF(#REF!=Q1,1,0)+IF(I32=Q1,1,0)+IF(I36=Q1,1,0)+IF(I40=Q1,1,0)+IF(I44=Q1,1,0)+IF(I48=Q1,1,0)+IF(I52=Q1,1,0)+IF(I56=Q1,1,0)+IF(I60=Q1,1,0)+IF(I64=Q1,1,0)+IF(I68=Q1,1,0)+IF(I72=Q1,1,0)+IF(I76=Q1,1,0)+IF(I80=Q1,1,0)+IF(I84=Q1,1,0)+IF(I88=Q1,1,0)+IF(I92=Q1,1,0)+IF(I96=Q1,1,0)+IF(I100=Q1,1,0)+IF(I101=Q1,1,0)+IF(I102=Q1,1,0)+IF(I103=Q1,1,0)</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="112" spans="1:10">
+      <c r="H112" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="I109" s="2"/>
+      <c r="I112" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="50">
-    <mergeCell ref="A101:A104"/>
-    <mergeCell ref="B101:B104"/>
-    <mergeCell ref="A85:A88"/>
-    <mergeCell ref="B85:B88"/>
-    <mergeCell ref="A89:A92"/>
-    <mergeCell ref="B89:B92"/>
-    <mergeCell ref="A93:A96"/>
-    <mergeCell ref="B93:B96"/>
-    <mergeCell ref="A77:A80"/>
-    <mergeCell ref="B77:B80"/>
-    <mergeCell ref="A81:A84"/>
-    <mergeCell ref="B81:B84"/>
-    <mergeCell ref="A97:A100"/>
-    <mergeCell ref="B97:B100"/>
-    <mergeCell ref="A65:A68"/>
-    <mergeCell ref="B65:B68"/>
-    <mergeCell ref="A69:A72"/>
-    <mergeCell ref="B69:B72"/>
-    <mergeCell ref="A73:A76"/>
-    <mergeCell ref="B73:B76"/>
-    <mergeCell ref="A53:A56"/>
-    <mergeCell ref="B53:B56"/>
-    <mergeCell ref="A57:A60"/>
-    <mergeCell ref="B57:B60"/>
-    <mergeCell ref="A61:A64"/>
-    <mergeCell ref="B61:B64"/>
-    <mergeCell ref="A41:A44"/>
-    <mergeCell ref="B41:B44"/>
-    <mergeCell ref="A45:A48"/>
-    <mergeCell ref="B45:B48"/>
-    <mergeCell ref="A49:A52"/>
-    <mergeCell ref="B49:B52"/>
-    <mergeCell ref="A29:A32"/>
-    <mergeCell ref="B29:B32"/>
-    <mergeCell ref="A33:A36"/>
-    <mergeCell ref="B33:B36"/>
-    <mergeCell ref="A37:A40"/>
-    <mergeCell ref="B37:B40"/>
-    <mergeCell ref="A17:A20"/>
-    <mergeCell ref="B17:B20"/>
-    <mergeCell ref="A21:A24"/>
-    <mergeCell ref="B21:B24"/>
-    <mergeCell ref="A25:A28"/>
-    <mergeCell ref="B25:B28"/>
+  <mergeCells count="56">
+    <mergeCell ref="C106:C107"/>
+    <mergeCell ref="D106:D107"/>
+    <mergeCell ref="E106:E107"/>
+    <mergeCell ref="F106:F107"/>
+    <mergeCell ref="B104:B108"/>
+    <mergeCell ref="A104:A108"/>
     <mergeCell ref="A3:A6"/>
     <mergeCell ref="B3:B6"/>
-    <mergeCell ref="B7:B10"/>
-    <mergeCell ref="A7:A10"/>
-    <mergeCell ref="B11:B16"/>
-    <mergeCell ref="A11:A16"/>
+    <mergeCell ref="B12:B17"/>
+    <mergeCell ref="A12:A17"/>
+    <mergeCell ref="A7:A11"/>
+    <mergeCell ref="B7:B11"/>
+    <mergeCell ref="A18:A21"/>
+    <mergeCell ref="B18:B21"/>
+    <mergeCell ref="A22:A25"/>
+    <mergeCell ref="B22:B25"/>
+    <mergeCell ref="A26:A29"/>
+    <mergeCell ref="B26:B29"/>
+    <mergeCell ref="A32:A35"/>
+    <mergeCell ref="B32:B35"/>
+    <mergeCell ref="A36:A39"/>
+    <mergeCell ref="B36:B39"/>
+    <mergeCell ref="A30:A31"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="A40:A43"/>
+    <mergeCell ref="B40:B43"/>
+    <mergeCell ref="A44:A47"/>
+    <mergeCell ref="B44:B47"/>
+    <mergeCell ref="A48:A51"/>
+    <mergeCell ref="B48:B51"/>
+    <mergeCell ref="A52:A55"/>
+    <mergeCell ref="B52:B55"/>
+    <mergeCell ref="A56:A59"/>
+    <mergeCell ref="B56:B59"/>
+    <mergeCell ref="A60:A63"/>
+    <mergeCell ref="B60:B63"/>
+    <mergeCell ref="A64:A67"/>
+    <mergeCell ref="B64:B67"/>
+    <mergeCell ref="A68:A71"/>
+    <mergeCell ref="B68:B71"/>
+    <mergeCell ref="A72:A75"/>
+    <mergeCell ref="B72:B75"/>
+    <mergeCell ref="A76:A79"/>
+    <mergeCell ref="B76:B79"/>
+    <mergeCell ref="A80:A83"/>
+    <mergeCell ref="B80:B83"/>
+    <mergeCell ref="A96:A99"/>
+    <mergeCell ref="B96:B99"/>
+    <mergeCell ref="A100:A103"/>
+    <mergeCell ref="B100:B103"/>
+    <mergeCell ref="A84:A87"/>
+    <mergeCell ref="B84:B87"/>
+    <mergeCell ref="A88:A91"/>
+    <mergeCell ref="B88:B91"/>
+    <mergeCell ref="A92:A95"/>
+    <mergeCell ref="B92:B95"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I3:I104">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I3:I108">
       <formula1>$P$1:$R$1</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>